<commit_message>
Changes in the examples
</commit_message>
<xml_diff>
--- a/inst/extdata/PDconsesus_file.xlsx
+++ b/inst/extdata/PDconsesus_file.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\tedma\OneDrive\Έγγραφα\itern\ProtE\inst\extdata\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{46C8EF7B-1FD7-4D56-ACDD-0A0C2A8CD183}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A6B36A3E-77BB-46D2-B185-C141B5F7038D}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="908" uniqueCount="662">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="796" uniqueCount="582">
   <si>
     <t>Checked</t>
   </si>
@@ -145,21 +145,6 @@
     <t>&gt;sp|P22599|A1AT2_MOUSE Alpha-1-antitrypsin 1-2 OS=Mus musculus OX=10090 GN=Serpina1b PE=1 SV=2</t>
   </si>
   <si>
-    <t>231</t>
-  </si>
-  <si>
-    <t>Q00896</t>
-  </si>
-  <si>
-    <t>Alpha-1-antitrypsin 1-3 OS=Mus musculus OX=10090 GN=Serpina1c PE=1 SV=2</t>
-  </si>
-  <si>
-    <t>MTPSISWGLLLLAGLCCLVPSFLAEDVQETDTSQKDQSPASHEIATNLGDFAISLYRELVHQSNTSNIFFSPVSIATAFAMLSLGSKGDTHTQILEGLQFNLTQTSEADIHKSFQHLLQTLNRPDSELQLSTGNGLFVNNDLKLVEKFLEEAKNHYQAEVFSVNFAESEEAKKVINDFVEKGTQGKIVEAVKKLDQDTVFALANYILFKGKWKKPFDPENTEEAEFHVDESTTVKVPMMTLSGMLDVHHCSTLSSWVLLMDYAGNATAVFLLPDDGKMQHLEQTLSKELISKFLLNRRRRLAQIHFPRLSISGEYNLKTLMSPLGITRIFNNGADLSGITEENAPLKLSQAVHKAVLTIDETGTEAAAVTVLLAVPYSMPPILRFDHPFLFIIFEEHTQSPLFVGKVVDPTH</t>
-  </si>
-  <si>
-    <t>&gt;sp|Q00896|A1AT3_MOUSE Alpha-1-antitrypsin 1-3 OS=Mus musculus OX=10090 GN=Serpina1c PE=1 SV=2</t>
-  </si>
-  <si>
     <t>69</t>
   </si>
   <si>
@@ -190,21 +175,6 @@
     <t>&gt;sp|Q00897|A1AT4_MOUSE Alpha-1-antitrypsin 1-4 OS=Mus musculus OX=10090 GN=Serpina1d PE=1 SV=1</t>
   </si>
   <si>
-    <t>225</t>
-  </si>
-  <si>
-    <t>Q91WP6</t>
-  </si>
-  <si>
-    <t>Serine protease inhibitor A3N OS=Mus musculus OX=10090 GN=Serpina3n PE=1 SV=1</t>
-  </si>
-  <si>
-    <t>MAFIAALGLLMAGICPAVLCFPDGTLGMDAAVQEDHDNGTQLDSLTLASINTDFAFSLYKELVLKNPDKNIVFSPLSISAALAVMSLGAKGNTLEEILEGLKFNLTETSEADIHQGFGHLLQRLNQPKDQVQISTGSALFIEKRQQILTEFQEKAKTLYQAEAFTADFQQPRQAKKLINDYVRKQTQGMIKELVSDLDKRTLMVLVNYIYFKAKWKVPFDPLDTFKSEFYAGKRRPVIVPMMSMEDLTTPYFRDEELSCTVVELKYTGNASALFILPDQGRMQQVEASLQPETLRKWKNSLKPRMIDELHLPKFSISTDYSLEDVLSKLGIREVFSTQADLSAITGTKDLRVSQVVHKAVLDVAETGTEAAAATGVKFVPMSAKLYPLTVYFNRPFLIMIFDTETEIAPFIAKIANPK</t>
-  </si>
-  <si>
-    <t>&gt;sp|Q91WP6|SPA3N_MOUSE Serine protease inhibitor A3N OS=Mus musculus OX=10090 GN=Serpina3n PE=1 SV=1</t>
-  </si>
-  <si>
     <t>24</t>
   </si>
   <si>
@@ -280,21 +250,6 @@
     <t>&gt;sp|Q06890|CLUS_MOUSE Clusterin OS=Mus musculus OX=10090 GN=Clu PE=1 SV=1</t>
   </si>
   <si>
-    <t>232</t>
-  </si>
-  <si>
-    <t>P19221</t>
-  </si>
-  <si>
-    <t>Prothrombin OS=Mus musculus OX=10090 GN=F2 PE=1 SV=1</t>
-  </si>
-  <si>
-    <t>MSHVRGLGLPGCLALAALVSLVHSQHVFLAPQQALSLLQRVRRANSGFLEELRKGNLERECVEEQCSYEEAFEALESPQDTDVFWAKYTVCDSVRKPRETFMDCLEGRCAMDLGVNYLGTVNVTHTGIQCQLWRSRYPHKPEINSTTHPGADLKENFCRNPDSSTTGPWCYTTDPTVRREECSVPVCGQEGRTTVVMTPRSGGSKDNLSPPLGQCLTERGRLYQGNLAVTTLGSPCLPWNSLPAKTLSKYQDFDPEVKLVENFCRNPDWDEEGAWCYVAGQPGDFEYCNLNYCEEAVGEENYDVDESIAGRTTDAEFHTFFNEKTFGLGEADCGLRPLFEKKSLKDTTEKELLDSYIDGRIVEGWDAEKGIAPWQVMLFRKSPQELLCGASLISDRWVLTAAHCILYPPWDKNFTENDLLVRIGKHSRTRYERNVEKISMLEKIYVHPRYNWRENLDRDIALLKLKKPVPFSDYIHPVCLPDKQTVTSLLRAGYKGRVTGWGNLRETWTTNINEIQPSVLQVVNLPIVERPVCKASTRIRITDNMFCAGFKVNDTKRGDACEGDSGGPFVMKSPFNNRWYQMGIVSWGEGCDRKGKYGFYTHVFRLKRWIQKVIDQFG</t>
-  </si>
-  <si>
-    <t>&gt;sp|P19221|THRB_MOUSE Prothrombin OS=Mus musculus OX=10090 GN=F2 PE=1 SV=1</t>
-  </si>
-  <si>
     <t>77</t>
   </si>
   <si>
@@ -325,21 +280,6 @@
     <t>&gt;sp|P01872|IGHM_MOUSE Immunoglobulin heavy constant mu OS=Mus musculus OX=10090 GN=Ighm PE=1 SV=2</t>
   </si>
   <si>
-    <t>233</t>
-  </si>
-  <si>
-    <t>O88783</t>
-  </si>
-  <si>
-    <t>Coagulation factor V OS=Mus musculus OX=10090 GN=F5 PE=1 SV=1</t>
-  </si>
-  <si>
-    <t>MLLVCPCFFLLVVLGTRWAGWGSHQAEAAQLRQFYVAAQGILWNYHPEPTDPSLNSIPSFKKIVYREYEQYFKKEKPRSSNSGLLGPTLYAEVGDVIKVHFRNKADKPLSIHPQGIKYSKFSEGASYADHTFPAERKDDAVAPGEEYTYEWIVSEDSGPTPDDPPCLTHIYYSYENLTQDFNSGLIGPLLICKKGTLTEDGTQKMFDKQHVLLFAVFDESKSRSQSPSLMYTINGFVNKTMPDITVCAHDHVSWHLIGMSSGPELFSIHFNGQVLEQNQHKVSTVTLVSATSTTANMTMSPEGRWIVSSLIPKHYQAGMQAYIDIKNCPKKTRSPKTLTREQRRYMKRWEYFIAAEEVIWNYAPVIPANMDKIYRSQHLDNFSNQIGKHYKKVIYRQYEEETFTKRTDNPSIKQSGILGPVIRAQVRDTLKIVFKNMASRPYSIYPHGVTFSPYEDGINSSSTSGSHTTIRPVQPGETFTYKWNILEFDEPTENDAQCLTRPYYSDVDVTRDIASGLIGLLLICKSRSLDQRGVQRVADIEQQAVFAVFDENKSWYIEDNINKFCENPDEVKRDDPKFYESNIMSTINGYVPESISTLGFCFDDTVQWHFCSVGTHDDILTIHFTGHSFIYGRRHEDTLTLFPMRGESVTVTMDNVGTWMLTTMNSNPKRRNLRLRFRDVKCNRDYDNEDSYEIYEPPAPTSMTTRRIHDSLENEFGIDNEDDDYQYLLASSLGIRSFKNSSLNPEENEFNLTALALENSSEFISPSTDRVVDSNSSRILSKIINNNLKDFQRTLPGSGATVAGTLLRNLIGLDENFVLNSSTEHRSSSYHENDMENPQSNITMVYLLPLGPKGSGNREQDKPKTIKTGRPHMMKHRFSWMKAPAGKTGRHSNPKNSYSGMKSEEDIPSELIPLKQKITSKFLNRRWRVASEKGSYEIIAANGEDTDVDKLTNSPQNQNITVPRGESTSHTNTTRKPSDLPTFSGVGHKSPHVRQEEENSGFQKRQLFIRTRKKKKNKKLALHSPLSPRGFDPLRGHNHSPFPDRRLLNHSLLLHKSNETALSPDLNQTSPSMSTDRSLPDYNQYSKNDTEQMSSSLDLYQSVPAEEHSPTFPAQDPDQTHSTTDPSYRSSPPELSQGLDYDLSHDFYPDDIGLTSFFPDQSQKSSFSSDDDQAIPSSDLSLFTISPELDQTIIYPDLDQLLLSPEDNQKTSSPDLGQVPLSPDDNQKTSSPDLGQVSLSPDDNQKTSSPDLGQVPLSLDDNQKTTSPDLGQVPLSPDDNQMITSPDLGQVPLSSDNQKTSSPDLGQVPLFPEDNQNYFLDLSQVPLSSDQNQETSSTDLLTLSPDFGQTVLSPDLDQLPLPSDNSQVTVSPDLSLLTLSPDFNEIILAPDLGQVTLSPDLIQTNPALNHGHKASSADPDQASYPPDSGQASSLPELNRTLPHPDLTHIPPPSPSPTLNNTSLSRKFNPLVVVGLSRVDGDDVEIVPSEEPERIDEDYAEDDFVTYNDPYRTDTRTDVNSSRNPDTIAAWYLRGHGGHKKFYYIAAEEITWNYAEFAQSEMDHEDTGHTPKDTTYKKVVFRKYLDSTFTSRDPRAEYEEHLGILGPVIRAEVDDVIQVRFKNLASRPYSLHAHGLSYEKSSEGKTYEDESPEWFQEDDAVQPNSSYTYVWHATKRSGPENPGSACRAWAYYSAVNVERDIHSGLIGPLLICRKGTLHMERNLPMDMREFVLLFMVFDEKKSWYYEKSKGSRRIESPEEKNAHKFYAINGMIYNLPGLRMYEQEWVRLHLLNMGGSRDIHVVHFHGQTLLDNRTKQHQLGVWPLLPGSFKTLEMKASKPGWWLLDTEVGENQVAGMQTPFLIIDKECKMPMGLSTGVISDSQIKASEYLTYWEPRLARLNNAGSYNAWSIEKTALDFPIKPWIQVDMQKEVVVTGIQTQGAKHYLKSCFTTEFQVAYSSDQTNWQIFRGKSGKSVMYFTGNSDGSTIKENRLDPPIVARYIRIHPTKSYNRPTLRLELQGCEVNGCSTPLGLEDGRIQDKQITASSFKKSWWGDYWEPSLARLNAQGRVNAWQAKANNNKQWLQVDLLKIKKVTAIVTQGCKSLSSEMYVKSYSIQYSDQGVAWKPYRQKSSMVDKIFEGNSNTKGHMKNFFNPPIISRFIRIIPKTWNQSIALRLELFGCDIY</t>
-  </si>
-  <si>
-    <t>&gt;sp|O88783|FA5_MOUSE Coagulation factor V OS=Mus musculus OX=10090 GN=F5 PE=1 SV=1</t>
-  </si>
-  <si>
     <t>83</t>
   </si>
   <si>
@@ -355,21 +295,6 @@
     <t>&gt;sp|Q8K182|CO8A_MOUSE Complement component C8 alpha chain OS=Mus musculus OX=10090 GN=C8a PE=1 SV=1</t>
   </si>
   <si>
-    <t>228</t>
-  </si>
-  <si>
-    <t>O70362</t>
-  </si>
-  <si>
-    <t>Phosphatidylinositol-glycan-specific phospholipase D OS=Mus musculus OX=10090 GN=Gpld1 PE=1 SV=1</t>
-  </si>
-  <si>
-    <t>MSAGRLWSSLLLLLPLFCSKSSSCGLSTHVEIGHRALEFLRLQDGRINYKELILEHQDAYQAGTVFPDAFYPSICKRGKYHDVSERTHWTPFLNASIHYIRENYPLPWEKDTEKLVAFLFGITSHMVADLSWHNLGFLRTMGAIDFYNSYSDAHSAGDFGGDVLSQFEFNFNYLSRRWYVPVRDLLRIYDNLYGRKVITKDVLVDCTYLQFLEMHGEMFAVSKLYSTYSTKSPFLVEQFQDYFLGGLDDMAFWSTNIYRLTSFMLENGTSDCNLPENPLFISCDGRNHTLSGSKVQKNDFHRNLTMFISRDIRKNLNYTERGVFYSTGSWARPESVTFMYQTLERNLRLMLAGSSQKNLNHVSSPSASYTLSVPYARLGWVMTSADLNQDGHGDLVVGAPGYSHPGRFQIGRVYIIYGNDLGLPPIDLDLNKEGILEGFQPSGRFGSALAVLDFNQDGLPDLAVGAPSVGSGQLTYNGSVYVYYGSQQGRLSSSPNVTISCKDTYCNLGWTLLATDADGDGRHDLVISSPFAPGGRKQKGIVATFYSHPRRNDKELLTLEEADWKVNGEEDFSWFGYSLHGVTVANRSLLLIGSPTWKNVSRMARSSHKKNQEEKSLGKVYGYFLPNRQSTITISGDKAMGKLGTSLSSGYVRVNGTLTQVLLVGAPTHDDVSKMAFLTMTLHQGGATRMYELAPEKTQPALLSTFSGDRRFSRFGSVLHLTDLDDDGLDEIIMAAPLRITDVTSGLLGGEDGRVYIYNGMYTTLGDMTGKCKSWMTPCPEEKAQYVLTSPEASSRFGSSLVSVRSKGRNQVVVAAGRSSWGARLSGALHVYSFSSD</t>
-  </si>
-  <si>
-    <t>&gt;sp|O70362|PHLD_MOUSE Phosphatidylinositol-glycan-specific phospholipase D OS=Mus musculus OX=10090 GN=Gpld1 PE=1 SV=1</t>
-  </si>
-  <si>
     <t>6</t>
   </si>
   <si>
@@ -460,21 +385,6 @@
     <t>&gt;sp|P03987|IGHG3_MOUSE Ig gamma-3 chain C region OS=Mus musculus OX=10090 PE=1 SV=2</t>
   </si>
   <si>
-    <t>223</t>
-  </si>
-  <si>
-    <t>Q60590</t>
-  </si>
-  <si>
-    <t>Alpha-1-acid glycoprotein 1 OS=Mus musculus OX=10090 GN=Orm1 PE=1 SV=1</t>
-  </si>
-  <si>
-    <t>MALHTVLIILSLLPMLEAQNPEHANFTIGEPITNETLSWLSDKWFFMGAAFRKLEYRQAIQTMQSEFFYLTTNLINDTIELRESQTIGDQCVYNSTHLGFQRENGTFSKYEGGVETFAHLIVLRKHGAFMLAFDLKDEKKRGLSLYAKRPDITPELREVFQKAVTHVGMDESEIIFVDWKKDRCGQQEKKQLELGKETKKDPEEGQA</t>
-  </si>
-  <si>
-    <t>&gt;sp|Q60590|A1AG1_MOUSE Alpha-1-acid glycoprotein 1 OS=Mus musculus OX=10090 GN=Orm1 PE=1 SV=1</t>
-  </si>
-  <si>
     <t>59</t>
   </si>
   <si>
@@ -520,21 +430,6 @@
     <t>&gt;sp|Q9DBB9|CPN2_MOUSE Carboxypeptidase N subunit 2 OS=Mus musculus OX=10090 GN=Cpn2 PE=1 SV=2</t>
   </si>
   <si>
-    <t>229</t>
-  </si>
-  <si>
-    <t>P31532</t>
-  </si>
-  <si>
-    <t>Serum amyloid A-4 protein OS=Mus musculus OX=10090 GN=Saa4 PE=1 SV=2</t>
-  </si>
-  <si>
-    <t>MRLATVIVLCSLFLGVSGDGWYSFFREAVQGTWDLWRAYRDNLEANYQNADQYFYARGNYEAQQRGSGGIWAAKIISTSRKYFQGLLNRYYFGIRNHGLETLQATQKAEEWGRSGKNPNHFRPEGLPEKF</t>
-  </si>
-  <si>
-    <t>&gt;sp|P31532|SAA4_MOUSE Serum amyloid A-4 protein OS=Mus musculus OX=10090 GN=Saa4 PE=1 SV=2</t>
-  </si>
-  <si>
     <t>45</t>
   </si>
   <si>
@@ -550,21 +445,6 @@
     <t>&gt;sp|Q8CG16|C1RA_MOUSE Complement C1r-A subcomponent OS=Mus musculus OX=10090 GN=C1ra PE=1 SV=1</t>
   </si>
   <si>
-    <t>22</t>
-  </si>
-  <si>
-    <t>Q8BND5</t>
-  </si>
-  <si>
-    <t>Sulfhydryl oxidase 1 OS=Mus musculus OX=10090 GN=Qsox1 PE=1 SV=1</t>
-  </si>
-  <si>
-    <t>MRRCGRLSGPPSLLLLLLLLSPLLFSGPGAYAARLSVLYSSSDPLTLLDADSVRPTVLGSSSAWAVEFFASWCGHCIAFAPTWKELANDVKDWRPALNLAVLDCAEETNSAVCREFNIAGFPTVRFFQAFTKNGSGATLPGAGANVQTLRMRLIDALESHRDTWPPACPPLEPAKLNDIDGFFTRNKADYLALVFEREDSYLGREVTLDLSQYHAVAVRRVLNTESDLVNKFGVTDFPSCYLLLRNGSVSRVPVLVESRSFYTSYLRGLPGLTRDAPPTTATPVTADKIAPTVWKFADRSKIYMADLESALHYILRVEVGKFSVLEGQRLVALKKFVAVLAKYFPGQPLVQNFLHSINDWLQKQQKKRIPYSFFKAALDSRKEDAVLTEKVNWVGCQGSEPHFRGFPCSLWVLFHFLTVQANRYSEAHPQEPADGQEVLQAMRSYVQFFFGCRDCADHFEQMAAASMHQVRSPSNAILWLWTSHNRVNARLSGALSEDPHFPKVQWPPRELCSACHNELNGQVPLWDLGATLNFLKAHFSPANIVIDSSASRHTGRRGSPEATPELVMDTLKLESRNSVLGHEQAASAESPGATALDVPAEKPEASGPQELYTGLRMGGASPGQGPPERMEDHQRDMQENAPGQQHLSKRDTEALFLPEVNHLQGPLELRRGGRSPKQLAPILEEEPEALAIQGQGQWLQVLGGGISHLDISLCVGLYSVSFMGLLAMYTYFRARLRTPKGHASYPTA</t>
-  </si>
-  <si>
-    <t>&gt;sp|Q8BND5|QSOX1_MOUSE Sulfhydryl oxidase 1 OS=Mus musculus OX=10090 GN=Qsox1 PE=1 SV=1</t>
-  </si>
-  <si>
     <t>36</t>
   </si>
   <si>
@@ -895,21 +775,6 @@
     <t>&gt;sp|P98086|C1QA_MOUSE Complement C1q subcomponent subunit A OS=Mus musculus OX=10090 GN=C1qa PE=1 SV=2</t>
   </si>
   <si>
-    <t>222</t>
-  </si>
-  <si>
-    <t>P51885</t>
-  </si>
-  <si>
-    <t>Lumican OS=Mus musculus OX=10090 GN=Lum PE=1 SV=2</t>
-  </si>
-  <si>
-    <t>MNVCAFSLALALVGSVSGQYYDYDIPLFMYGQISPNCAPECNCPHSYPTAMYCDDLKLKSVPMVPPGIKYLYLRNNQIDHIDEKAFENVTDLQWLILDHNLLENSKIKGKVFSKLKQLKKLHINYNNLTESVGPLPKSLQDLQLTNNKISKLGSFDGLVNLTFIYLQHNQLKEDAVSASLKGLKSLEYLDLSFNQMSKLPAGLPTSLLTLYLDNNKISNIPDEYFKRFTGLQYLRLSHNELADSGVPGNSFNISSLLELDLSYNKLKSIPTVNENLENYYLEVNELEKFDVKSFCKILGPLSYSKIKHLRLDGNPLTQSSLPPDMYECLRVANEITVN</t>
-  </si>
-  <si>
-    <t>&gt;sp|P51885|LUM_MOUSE Lumican OS=Mus musculus OX=10090 GN=Lum PE=1 SV=2</t>
-  </si>
-  <si>
     <t>72</t>
   </si>
   <si>
@@ -940,21 +805,6 @@
     <t>&gt;sp|P41317|MBL2_MOUSE Mannose-binding protein C OS=Mus musculus OX=10090 GN=Mbl2 PE=1 SV=2</t>
   </si>
   <si>
-    <t>230</t>
-  </si>
-  <si>
-    <t>Q61171</t>
-  </si>
-  <si>
-    <t>Peroxiredoxin-2 OS=Mus musculus OX=10090 GN=Prdx2 PE=1 SV=3</t>
-  </si>
-  <si>
-    <t>MASGNAQIGKSAPDFTATAVVDGAFKEIKLSDYRGKYVVLFFYPLDFTFVCPTEIIAFSDHAEDFRKLGCEVLGVSVDSQFTHLAWINTPRKEGGLGPLNIPLLADVTKSLSQNYGVLKNDEGIAYRGLFIIDAKGVLRQITVNDLPVGRSVDEALRLVQAFQYTDEHGEVCPAGWKPGSDTIKPNVDDSKEYFSKHN</t>
-  </si>
-  <si>
-    <t>&gt;sp|Q61171|PRDX2_MOUSE Peroxiredoxin-2 OS=Mus musculus OX=10090 GN=Prdx2 PE=1 SV=3</t>
-  </si>
-  <si>
     <t>92</t>
   </si>
   <si>
@@ -1045,21 +895,6 @@
     <t>&gt;sp|Q02105|C1QC_MOUSE Complement C1q subcomponent subunit C OS=Mus musculus OX=10090 GN=C1qc PE=1 SV=2</t>
   </si>
   <si>
-    <t>226</t>
-  </si>
-  <si>
-    <t>P01864</t>
-  </si>
-  <si>
-    <t>Ig gamma-2A chain C region secreted form OS=Mus musculus OX=10090 PE=1 SV=1</t>
-  </si>
-  <si>
-    <t>AKTTAPSVYPLVPVCGGTTGSSVTLGCLVKGYFPEPVTLTWNSGSLSSGVHTFPALLQSGLYTLSSSVTVTSNTWPSQTITCNVAHPASSTKVDKKIEPRVPITQNPCPPHQRVPPCAAPDLLGGPSVFIFPPKIKDVLMISLSPMVTCVVVDVSEDDPDVQISWFVNNVEVHTAQTQTHREDYNSTLRVVSALPIQHQDWMSGKEFKCKVNNRALPSPIEKTISKPRGPVRAPQVYVLPPPAEEMTKKEFSLTCMITGFLPAEIAVDWTSNGRTEQNYKNTATVLDSDGSYFMYSKLRVQKSTWERGSLFACSVVHEVLHNHLTTKTISRSLGK</t>
-  </si>
-  <si>
-    <t>&gt;sp|P01864|GCAB_MOUSE Ig gamma-2A chain C region secreted form OS=Mus musculus OX=10090 PE=1 SV=1</t>
-  </si>
-  <si>
     <t>91</t>
   </si>
   <si>
@@ -1270,36 +1105,6 @@
     <t>&gt;sp|P01807|HVM37_MOUSE Ig heavy chain V region X44 OS=Mus musculus OX=10090 PE=1 SV=1</t>
   </si>
   <si>
-    <t>23</t>
-  </si>
-  <si>
-    <t>P01800</t>
-  </si>
-  <si>
-    <t>Ig heavy chain V-III region T957 OS=Mus musculus OX=10090 PE=1 SV=2</t>
-  </si>
-  <si>
-    <t>EVKLEESGGGLVQPGGSMKLSCVASGFTFSNYWMNWVRQSPEKGLEWVAEIRLKSHNYETHYAESVKGRFTISRDDSKSSVYLQMNILRAEDTGIYYCTTGFAYWGQGTLVTV</t>
-  </si>
-  <si>
-    <t>&gt;sp|P01800|HVM31_MOUSE Ig heavy chain V-III region T957 OS=Mus musculus OX=10090 PE=1 SV=2</t>
-  </si>
-  <si>
-    <t>220</t>
-  </si>
-  <si>
-    <t>Q6GQT1</t>
-  </si>
-  <si>
-    <t>Alpha-2-macroglobulin-P OS=Mus musculus OX=10090 GN=A2m PE=2 SV=2</t>
-  </si>
-  <si>
-    <t>MGKRWLPSLALLPLPPPLLLLLLLLLPTNASAPQKPIYMVMVPSLLHAGTPEKGCLLFNHLNETVTVKVSMESVRGNQSLFTDLVVDKDLFHCASFIVPQSSSNEVMFLTVQVKGPTHEFRRRSTVLIKTKESLVFAQTDKPIYKPGQMVRFRVVSLDENFHPLNELIPLLYIQDSKKNRIAQWQNFRLEGGLKQLSFPLSSEPTQGSYKVVIRTESGRTVEHPFSVKEFVLPKFEVKVAVPETITILEEEMNVSVCGIYTYGKPVPGHVTVNICRKYSNPSSCFGEESLAFCEKFSQQLDGRGCFSQLVKTKSFQLKRQEYEMQLDVNAKIQEEGTGVEETGKGLTKITRTITKLSFVNVDTHFRQGIPFVGQVLLVDGRGTPIPYEMIFIGADEANQNINTTTDKNGLARFSINTDDIMGTSLTVRAKYKDSNVCYGFRWLTEENVEAWHTANAVFSPSRSFVHLESLPYKLRCEQTLAVQAHYILNDEAVLERKELVFYYLMMAKGGIVRAGTHVLPVTQGHKKGHFSILISMETDLAPVARLVLYTILPNGEVVGDTVKYEIEKCLANKVDLVFHPNIGLPATRAFLSVMASPQSLCGLRAVDQSVLLTKPEAELSASLVYDLLPVKDLTGFPKGVNQQEEDTNGCLKQNDTYINGILYSPVQNTNEEDMYGFLKDMGLKVFTNLNIRKPKVCERLGVNKIPAAYHLVSQGHMDAFLESSESPTETTRSYFPETWIWDLVIVDSTGVAEMEVTVPDTITEWKAGAFCLSNDTGLGLSPVIDFQAFQPFFVDLTMPYSVIRGEAFTLKATVLNYLQTCIRVGVQLEASPDFLATPEEKEQKSHCICMNERHTMSWAVIPKSLGNVNFTVSAEALDSKELCRNEVPVVPERGKKDTIIKSLLVEPEGLENEVTFNSLLCPTGAEVSEQISLKLPSDVVEESARASVTVLGDILGSAMQNTQDLLKMPYGCGEQNMVLFAPNIYVLDYLNETEQLTQEIKTKAITYLNTGYQRQLNYKHRDGSYSTFGDKPGRSHANTWLTAFVLKSFAQARRYIFIDESHITQALTWLSQQQKDNGCFRSSGSLLNNAMKGGVEDEVTLSAYITIALLEMSLPVTHPVVRNALFCLDTAWKSARRGASGNHVYTKALLAYAFALAGNQDTKKEILKSLDEEAVKEDNSVHWTRAQKPRVPADLWYQPQAPSAEVEMTAYVLLAYLTTELVPTREDLTAAMLIVKWLTKQQNSHGGFSSTQDTVVALHALSKYGAATFTRAKKAAHVTIQSSGAFYTKFQVNNDNQLLLQRVTLPTVPGDYTAKVAGEGCVYLQTSLKYSVLPREKEFPFALVVQTLPGTCEDLKAHTTFQISLNISYIGSRSDSNMAIADVKMVSGFIPLKPTVKMLERSVHVSRTEVSNNHVLIYLDKVSNQMLTLFFMVQQDIPVRDLKPAIVKVYDYYEKDEFAVAKYSAPCSAGYGNA</t>
-  </si>
-  <si>
-    <t>&gt;sp|Q6GQT1|A2MG_MOUSE Alpha-2-macroglobulin-P OS=Mus musculus OX=10090 GN=A2m PE=2 SV=2</t>
-  </si>
-  <si>
     <t>75</t>
   </si>
   <si>
@@ -1345,21 +1150,6 @@
     <t>&gt;sp|Q61696|HS71A_MOUSE Heat shock 70 kDa protein 1A OS=Mus musculus OX=10090 GN=Hspa1a PE=1 SV=2</t>
   </si>
   <si>
-    <t>224</t>
-  </si>
-  <si>
-    <t>P62827</t>
-  </si>
-  <si>
-    <t>GTP-binding nuclear protein Ran OS=Mus musculus OX=10090 GN=Ran PE=1 SV=3</t>
-  </si>
-  <si>
-    <t>MAAQGEPQVQFKLVLVGDGGTGKTTFVKRHLTGEFEKKYVATLGVEVHPLVFHTNRGPIKFNVWDTAGQEKFGGLRDGYYIQAQCAIIMFDVTSRVTYKNVPNWHRDLVRVCENIPIVLCGNKVDIKDRKVKAKSIVFHRKKNLQYYDISAKSNYNFEKPFLWLARKLIGDPNLEFVAMPALAPPEVVMDPALAAQYEHDLEVAQTTALPDEDDDL</t>
-  </si>
-  <si>
-    <t>&gt;sp|P62827|RAN_MOUSE GTP-binding nuclear protein Ran OS=Mus musculus OX=10090 GN=Ran PE=1 SV=3</t>
-  </si>
-  <si>
     <t>61</t>
   </si>
   <si>
@@ -1645,21 +1435,6 @@
     <t>&gt;sp|P26928|HGFL_MOUSE Hepatocyte growth factor-like protein OS=Mus musculus OX=10090 GN=Mst1 PE=2 SV=2</t>
   </si>
   <si>
-    <t>227</t>
-  </si>
-  <si>
-    <t>P11087</t>
-  </si>
-  <si>
-    <t>Collagen alpha-1(I) chain OS=Mus musculus OX=10090 GN=Col1a1 PE=1 SV=4</t>
-  </si>
-  <si>
-    <t>MFSFVDLRLLLLLGATALLTHGQEDIPEVSCIHNGLRVPNGETWKPEVCLICICHNGTAVCDDVQCNEELDCPNPQRREGECCAFCPEEYVSPNSEDVGVEGPKGDPGPQGPRGPVGPPGRDGIPGQPGLPGPPGPPGPPGPPGLGGNFASQMSYGYDEKSAGVSVPGPMGPSGPRGLPGPPGAPGPQGFQGPPGEPGEPGGSGPMGPRGPPGPPGKNGDDGEAGKPGRPGERGPPGPQGARGLPGTAGLPGMKGHRGFSGLDGAKGDAGPAGPKGEPGSPGENGAPGQMGPRGLPGERGRPGPPGTAGARGNDGAVGAAGPPGPTGPTGPPGFPGAVGAKGEAGPQGARGSEGPQGVRGEPGPPGPAGAAGPAGNPGADGQPGAKGANGAPGIAGAPGFPGARGPSGPQGPSGPPGPKGNSGEPGAPGNKGDTGAKGEPGATGVQGPPGPAGEEGKRGARGEPGPSGLPGPPGERGGPGSRGFPGADGVAGPKGPSGERGAPGPAGPKGSPGEAGRPGEAGLPGAKGLTGSPGSPGPDGKTGPPGPAGQDGRPGPAGPPGARGQAGVMGFPGPKGTAGEPGKAGERGLPGPPGAVGPAGKDGEAGAQGAPGPAGPAGERGEQGPAGSPGFQGLPGPAGPPGEAGKPGEQGVPGDLGAPGPSGARGERGFPGERGVQGPPGPAGPRGNNGAPGNDGAKGDTGAPGAPGSQGAPGLQGMPGERGAAGLPGPKGDRGDAGPKGADGSPGKDGARGLTGPIGPPGPAGAPGDKGEAGPSGPPGPTGARGAPGDRGEAGPPGPAGFAGPPGADGQPGAKGEPGDTGVKGDAGPPGPAGPAGPPGPIGNVGAPGPKGPRGAAGPPGATGFPGAAGRVGPPGPSGNAGPPGPPGPVGKEGGKGPRGETGPAGRPGEVGPPGPPGPAGEKGSPGADGPAGSPGTPGPQGIAGQRGVVGLPGQRGERGFPGLPGPSGEPGKQGPSGSSGERGPPGPMGPPGLAGPPGESGREGSPGAEGSPGRDGAPGAKGDRGETGPAGPPGAPGAPGAPGPVGPAGKNGDRGETGPAGPAGPIGPAGARGPAGPQGPRGDKGETGEQGDRGIKGHRGFSGLQGPPGSPGSPGEQGPSGASGPAGPRGPPGSAGSPGKDGLNGLPGPIGPPGPRGRTGDSGPAGPPGPPGPPGPPGPPSGGYDFSFLPQPPQEKSQDGGRYYRADDANVVRDRDLEVDTTLKSLSQQIENIRSPEGSRKNPARTCRDLKMCHSDWKSGEYWIDPNQGCNLDAIKVYCNMETGQTCVFPTQPSVPQKNWYISPNPKEKKHVWFGESMTDGFPFEYGSEGSDPADVAIQLTFLRLMSTEASQNITYHCKNSVAYMDQQTGNLKKALLLQGSNEIELRGEGNSRFTYSTLVDGCTSHTGTWGKTVIEYKTTKTSRLPIIDVAPLDIGAPDQEFGLDIGPACFV</t>
-  </si>
-  <si>
-    <t>&gt;sp|P11087|CO1A1_MOUSE Collagen alpha-1(I) chain OS=Mus musculus OX=10090 GN=Col1a1 PE=1 SV=4</t>
-  </si>
-  <si>
     <t>56</t>
   </si>
   <si>
@@ -1928,21 +1703,6 @@
   </si>
   <si>
     <t>&gt;sp|O35231|KIFC3_MOUSE Kinesin-like protein KIFC3 OS=Mus musculus OX=10090 GN=Kifc3 PE=1 SV=4</t>
-  </si>
-  <si>
-    <t>221</t>
-  </si>
-  <si>
-    <t>Q9CSH3</t>
-  </si>
-  <si>
-    <t>Exosome complex exonuclease RRP44 OS=Mus musculus OX=10090 GN=Dis3 PE=1 SV=4</t>
-  </si>
-  <si>
-    <t>MLRSKTFLKKTRAGGVVKIVREHYLRDDIGCGAPACSACGGAHAGPALELQPRDQASSLCPWPHYLLPDTNVLLHQIDVLEHPAIRNVIVLQTVMQEVRNRSAPIYKRIRDVTNNQEKHFYTFTNEHHKETYIEQEQGENANDRNDRAIRVAAKWYNEHLKRVAADSQLQVILITNDRKNKEKAVQEGIPAFTCEEYVKSLTANPELIDRLAYLSDEMNEIESGKIIFSEHLPLSKLQQGIKSGSYLQGTFRASRENYLEATVWIHGDKEEEKEILIQGIKHLNRAVHEDIVAVELLPRSQWVAPSSVVLDDEGQNEDDVEKDEERELLLKTAVSEKMLRPTGRVVGIIKRNWRPYCGMLSKSDIKESRRHLFTPADKRIPRIRIETRQASALEGRRIIVAIDGWPRNSRYPNGHFVKNLGDVGEKETETEVLLLEHDVPHQPFSQAVLSFLPRMPWSITEEDMKNREDLRHLCVCSVDPPGCTDIDDALHCRELSNGNLEVGVHIADVSHFIRPGNALDQESARRGTTVYLCEKRIDMVPELLSSNLCSLRSNVDRLAFSCIWEMNHNAEILKTRFTKSVINSKASLTYAEAQMRIDSAAMNDDITTSLRGLNQLAKILKKGRIEKGALTLSSPEIRFHMDSETHDPIDLQTKELRETNSMVEEFMLLANISVAKKIHEEFSEHALLRKHPAPPPSNYDILVKAAKSKNLQIKTDTAKSLADSLDRAESPDFPYLNTLLRILATRCMMQAVYFCSGMDNDFHHYGLASPIYTHFTSPIRRYADIIVHRLLAVAIGADCTYPELTDKHKLSDICKNLNFRHKMAQYAQRASVAFHTQLFFKSKGIVSEEAYILFVRKNAIVVLIPKYGLEGTVFFEEKDKPKPRLAYDDEIPSLRIEGTVFHVFDKVKVKITLDSSNLQHQKIRMALVEPQIPGINIPPNVADKALTAPGGKKRKLEK</t>
-  </si>
-  <si>
-    <t>&gt;sp|Q9CSH3|RRP44_MOUSE Exosome complex exonuclease RRP44 OS=Mus musculus OX=10090 GN=Dis3 PE=1 SV=4</t>
   </si>
   <si>
     <t>28</t>
@@ -2339,10 +2099,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:AN125"/>
+  <dimension ref="A1:AN109"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A126" sqref="A126:BD331"/>
+    <sheetView tabSelected="1" topLeftCell="AG109" workbookViewId="0">
+      <selection activeCell="AO129" sqref="A110:AO129"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11.5546875" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -2421,52 +2181,52 @@
         <v>23</v>
       </c>
       <c r="Y1" t="s">
-        <v>646</v>
+        <v>566</v>
       </c>
       <c r="Z1" t="s">
-        <v>647</v>
+        <v>567</v>
       </c>
       <c r="AA1" t="s">
-        <v>648</v>
+        <v>568</v>
       </c>
       <c r="AB1" t="s">
-        <v>649</v>
+        <v>569</v>
       </c>
       <c r="AC1" t="s">
-        <v>650</v>
+        <v>570</v>
       </c>
       <c r="AD1" t="s">
-        <v>653</v>
+        <v>573</v>
       </c>
       <c r="AE1" t="s">
-        <v>652</v>
+        <v>572</v>
       </c>
       <c r="AF1" t="s">
-        <v>651</v>
+        <v>571</v>
       </c>
       <c r="AG1" t="s">
-        <v>654</v>
+        <v>574</v>
       </c>
       <c r="AH1" t="s">
-        <v>655</v>
+        <v>575</v>
       </c>
       <c r="AI1" t="s">
-        <v>656</v>
+        <v>576</v>
       </c>
       <c r="AJ1" t="s">
-        <v>657</v>
+        <v>577</v>
       </c>
       <c r="AK1" t="s">
-        <v>658</v>
+        <v>578</v>
       </c>
       <c r="AL1" t="s">
-        <v>659</v>
+        <v>579</v>
       </c>
       <c r="AM1" t="s">
-        <v>660</v>
+        <v>580</v>
       </c>
       <c r="AN1" t="s">
-        <v>661</v>
+        <v>581</v>
       </c>
     </row>
     <row r="2" spans="1:40" x14ac:dyDescent="0.3">
@@ -2480,19 +2240,19 @@
         <v>25</v>
       </c>
       <c r="D2" t="s">
-        <v>221</v>
+        <v>181</v>
       </c>
       <c r="E2" t="s">
-        <v>222</v>
+        <v>182</v>
       </c>
       <c r="F2" t="s">
-        <v>223</v>
+        <v>183</v>
       </c>
       <c r="G2" t="s">
-        <v>224</v>
+        <v>184</v>
       </c>
       <c r="H2" t="s">
-        <v>225</v>
+        <v>185</v>
       </c>
       <c r="I2">
         <v>0</v>
@@ -2602,19 +2362,19 @@
         <v>25</v>
       </c>
       <c r="D3" t="s">
-        <v>206</v>
+        <v>166</v>
       </c>
       <c r="E3" t="s">
-        <v>207</v>
+        <v>167</v>
       </c>
       <c r="F3" t="s">
-        <v>208</v>
+        <v>168</v>
       </c>
       <c r="G3" t="s">
-        <v>209</v>
+        <v>169</v>
       </c>
       <c r="H3" t="s">
-        <v>210</v>
+        <v>170</v>
       </c>
       <c r="I3">
         <v>0</v>
@@ -2724,19 +2484,19 @@
         <v>25</v>
       </c>
       <c r="D4" t="s">
-        <v>506</v>
+        <v>436</v>
       </c>
       <c r="E4" t="s">
-        <v>507</v>
+        <v>437</v>
       </c>
       <c r="F4" t="s">
-        <v>508</v>
+        <v>438</v>
       </c>
       <c r="G4" t="s">
-        <v>509</v>
+        <v>439</v>
       </c>
       <c r="H4" t="s">
-        <v>510</v>
+        <v>440</v>
       </c>
       <c r="I4">
         <v>0</v>
@@ -2843,19 +2603,19 @@
         <v>25</v>
       </c>
       <c r="D5" t="s">
-        <v>511</v>
+        <v>441</v>
       </c>
       <c r="E5" t="s">
-        <v>512</v>
+        <v>442</v>
       </c>
       <c r="F5" t="s">
-        <v>513</v>
+        <v>443</v>
       </c>
       <c r="G5" t="s">
-        <v>514</v>
+        <v>444</v>
       </c>
       <c r="H5" t="s">
-        <v>515</v>
+        <v>445</v>
       </c>
       <c r="I5">
         <v>0</v>
@@ -2965,19 +2725,19 @@
         <v>25</v>
       </c>
       <c r="D6" t="s">
-        <v>501</v>
+        <v>431</v>
       </c>
       <c r="E6" t="s">
-        <v>502</v>
+        <v>432</v>
       </c>
       <c r="F6" t="s">
-        <v>503</v>
+        <v>433</v>
       </c>
       <c r="G6" t="s">
-        <v>504</v>
+        <v>434</v>
       </c>
       <c r="H6" t="s">
-        <v>505</v>
+        <v>435</v>
       </c>
       <c r="I6">
         <v>0</v>
@@ -3191,19 +2951,19 @@
         <v>25</v>
       </c>
       <c r="D8" t="s">
-        <v>311</v>
+        <v>261</v>
       </c>
       <c r="E8" t="s">
-        <v>312</v>
+        <v>262</v>
       </c>
       <c r="F8" t="s">
-        <v>313</v>
+        <v>263</v>
       </c>
       <c r="G8" t="s">
-        <v>314</v>
+        <v>264</v>
       </c>
       <c r="H8" t="s">
-        <v>315</v>
+        <v>265</v>
       </c>
       <c r="I8">
         <v>0</v>
@@ -3313,19 +3073,19 @@
         <v>25</v>
       </c>
       <c r="D9" t="s">
-        <v>346</v>
+        <v>291</v>
       </c>
       <c r="E9" t="s">
-        <v>347</v>
+        <v>292</v>
       </c>
       <c r="F9" t="s">
-        <v>348</v>
+        <v>293</v>
       </c>
       <c r="G9" t="s">
-        <v>349</v>
+        <v>294</v>
       </c>
       <c r="H9" t="s">
-        <v>350</v>
+        <v>295</v>
       </c>
       <c r="I9">
         <v>0</v>
@@ -3435,19 +3195,19 @@
         <v>25</v>
       </c>
       <c r="D10" t="s">
-        <v>301</v>
+        <v>256</v>
       </c>
       <c r="E10" t="s">
-        <v>302</v>
+        <v>257</v>
       </c>
       <c r="F10" t="s">
-        <v>303</v>
+        <v>258</v>
       </c>
       <c r="G10" t="s">
-        <v>304</v>
+        <v>259</v>
       </c>
       <c r="H10" t="s">
-        <v>305</v>
+        <v>260</v>
       </c>
       <c r="I10">
         <v>0</v>
@@ -3557,19 +3317,19 @@
         <v>25</v>
       </c>
       <c r="D11" t="s">
-        <v>331</v>
+        <v>281</v>
       </c>
       <c r="E11" t="s">
-        <v>332</v>
+        <v>282</v>
       </c>
       <c r="F11" t="s">
-        <v>333</v>
+        <v>283</v>
       </c>
       <c r="G11" t="s">
-        <v>334</v>
+        <v>284</v>
       </c>
       <c r="H11" t="s">
-        <v>335</v>
+        <v>285</v>
       </c>
       <c r="I11">
         <v>0</v>
@@ -3679,19 +3439,19 @@
         <v>25</v>
       </c>
       <c r="D12" t="s">
-        <v>141</v>
+        <v>116</v>
       </c>
       <c r="E12" t="s">
-        <v>142</v>
+        <v>117</v>
       </c>
       <c r="F12" t="s">
-        <v>143</v>
+        <v>118</v>
       </c>
       <c r="G12" t="s">
-        <v>144</v>
+        <v>119</v>
       </c>
       <c r="H12" t="s">
-        <v>145</v>
+        <v>120</v>
       </c>
       <c r="I12">
         <v>0</v>
@@ -3801,19 +3561,19 @@
         <v>25</v>
       </c>
       <c r="D13" t="s">
-        <v>591</v>
+        <v>516</v>
       </c>
       <c r="E13" t="s">
-        <v>592</v>
+        <v>517</v>
       </c>
       <c r="F13" t="s">
-        <v>593</v>
+        <v>518</v>
       </c>
       <c r="G13" t="s">
-        <v>594</v>
+        <v>519</v>
       </c>
       <c r="H13" t="s">
-        <v>595</v>
+        <v>520</v>
       </c>
       <c r="I13">
         <v>0</v>
@@ -3923,19 +3683,19 @@
         <v>25</v>
       </c>
       <c r="D14" t="s">
-        <v>611</v>
+        <v>536</v>
       </c>
       <c r="E14" t="s">
-        <v>612</v>
+        <v>537</v>
       </c>
       <c r="F14" t="s">
-        <v>613</v>
+        <v>538</v>
       </c>
       <c r="G14" t="s">
-        <v>614</v>
+        <v>539</v>
       </c>
       <c r="H14" t="s">
-        <v>615</v>
+        <v>540</v>
       </c>
       <c r="I14">
         <v>0</v>
@@ -4042,19 +3802,19 @@
         <v>25</v>
       </c>
       <c r="D15" t="s">
-        <v>461</v>
+        <v>391</v>
       </c>
       <c r="E15" t="s">
-        <v>462</v>
+        <v>392</v>
       </c>
       <c r="F15" t="s">
-        <v>463</v>
+        <v>393</v>
       </c>
       <c r="G15" t="s">
-        <v>464</v>
+        <v>394</v>
       </c>
       <c r="H15" t="s">
-        <v>465</v>
+        <v>395</v>
       </c>
       <c r="I15">
         <v>0</v>
@@ -4164,19 +3924,19 @@
         <v>25</v>
       </c>
       <c r="D16" t="s">
-        <v>616</v>
+        <v>541</v>
       </c>
       <c r="E16" t="s">
-        <v>617</v>
+        <v>542</v>
       </c>
       <c r="F16" t="s">
-        <v>618</v>
+        <v>543</v>
       </c>
       <c r="G16" t="s">
-        <v>619</v>
+        <v>544</v>
       </c>
       <c r="H16" t="s">
-        <v>620</v>
+        <v>545</v>
       </c>
       <c r="I16">
         <v>0</v>
@@ -4286,19 +4046,19 @@
         <v>25</v>
       </c>
       <c r="D17" t="s">
-        <v>231</v>
+        <v>191</v>
       </c>
       <c r="E17" t="s">
-        <v>232</v>
+        <v>192</v>
       </c>
       <c r="F17" t="s">
-        <v>233</v>
+        <v>193</v>
       </c>
       <c r="G17" t="s">
-        <v>234</v>
+        <v>194</v>
       </c>
       <c r="H17" t="s">
-        <v>235</v>
+        <v>195</v>
       </c>
       <c r="I17">
         <v>0</v>
@@ -4405,19 +4165,19 @@
         <v>25</v>
       </c>
       <c r="D18" t="s">
-        <v>106</v>
+        <v>86</v>
       </c>
       <c r="E18" t="s">
-        <v>107</v>
+        <v>87</v>
       </c>
       <c r="F18" t="s">
-        <v>108</v>
+        <v>88</v>
       </c>
       <c r="G18" t="s">
-        <v>109</v>
+        <v>89</v>
       </c>
       <c r="H18" t="s">
-        <v>110</v>
+        <v>90</v>
       </c>
       <c r="I18">
         <v>0</v>
@@ -4524,19 +4284,19 @@
         <v>25</v>
       </c>
       <c r="D19" t="s">
-        <v>566</v>
+        <v>491</v>
       </c>
       <c r="E19" t="s">
-        <v>567</v>
+        <v>492</v>
       </c>
       <c r="F19" t="s">
-        <v>568</v>
+        <v>493</v>
       </c>
       <c r="G19" t="s">
-        <v>569</v>
+        <v>494</v>
       </c>
       <c r="H19" t="s">
-        <v>570</v>
+        <v>495</v>
       </c>
       <c r="I19">
         <v>0</v>
@@ -4646,19 +4406,19 @@
         <v>25</v>
       </c>
       <c r="D20" t="s">
-        <v>261</v>
+        <v>221</v>
       </c>
       <c r="E20" t="s">
-        <v>262</v>
+        <v>222</v>
       </c>
       <c r="F20" t="s">
-        <v>263</v>
+        <v>223</v>
       </c>
       <c r="G20" t="s">
-        <v>264</v>
+        <v>224</v>
       </c>
       <c r="H20" t="s">
-        <v>265</v>
+        <v>225</v>
       </c>
       <c r="I20">
         <v>0</v>
@@ -4768,19 +4528,19 @@
         <v>25</v>
       </c>
       <c r="D21" t="s">
-        <v>431</v>
+        <v>366</v>
       </c>
       <c r="E21" t="s">
-        <v>432</v>
+        <v>367</v>
       </c>
       <c r="F21" t="s">
-        <v>433</v>
+        <v>368</v>
       </c>
       <c r="G21" t="s">
-        <v>434</v>
+        <v>369</v>
       </c>
       <c r="H21" t="s">
-        <v>435</v>
+        <v>370</v>
       </c>
       <c r="I21">
         <v>0</v>
@@ -4890,19 +4650,19 @@
         <v>25</v>
       </c>
       <c r="D22" t="s">
-        <v>211</v>
+        <v>171</v>
       </c>
       <c r="E22" t="s">
-        <v>212</v>
+        <v>172</v>
       </c>
       <c r="F22" t="s">
-        <v>213</v>
+        <v>173</v>
       </c>
       <c r="G22" t="s">
-        <v>214</v>
+        <v>174</v>
       </c>
       <c r="H22" t="s">
-        <v>215</v>
+        <v>175</v>
       </c>
       <c r="I22">
         <v>0</v>
@@ -5012,19 +4772,19 @@
         <v>25</v>
       </c>
       <c r="D23" t="s">
-        <v>96</v>
+        <v>81</v>
       </c>
       <c r="E23" t="s">
-        <v>97</v>
+        <v>82</v>
       </c>
       <c r="F23" t="s">
-        <v>98</v>
+        <v>83</v>
       </c>
       <c r="G23" t="s">
-        <v>99</v>
+        <v>84</v>
       </c>
       <c r="H23" t="s">
-        <v>100</v>
+        <v>85</v>
       </c>
       <c r="I23">
         <v>0</v>
@@ -5256,19 +5016,19 @@
         <v>25</v>
       </c>
       <c r="D25" t="s">
-        <v>91</v>
+        <v>76</v>
       </c>
       <c r="E25" t="s">
-        <v>92</v>
+        <v>77</v>
       </c>
       <c r="F25" t="s">
-        <v>93</v>
+        <v>78</v>
       </c>
       <c r="G25" t="s">
-        <v>94</v>
+        <v>79</v>
       </c>
       <c r="H25" t="s">
-        <v>95</v>
+        <v>80</v>
       </c>
       <c r="I25">
         <v>0</v>
@@ -5378,19 +5138,19 @@
         <v>25</v>
       </c>
       <c r="D26" t="s">
-        <v>471</v>
+        <v>401</v>
       </c>
       <c r="E26" t="s">
-        <v>472</v>
+        <v>402</v>
       </c>
       <c r="F26" t="s">
-        <v>473</v>
+        <v>403</v>
       </c>
       <c r="G26" t="s">
-        <v>474</v>
+        <v>404</v>
       </c>
       <c r="H26" t="s">
-        <v>475</v>
+        <v>405</v>
       </c>
       <c r="I26">
         <v>0</v>
@@ -5500,19 +5260,19 @@
         <v>25</v>
       </c>
       <c r="D27" t="s">
-        <v>426</v>
+        <v>361</v>
       </c>
       <c r="E27" t="s">
-        <v>427</v>
+        <v>362</v>
       </c>
       <c r="F27" t="s">
-        <v>428</v>
+        <v>363</v>
       </c>
       <c r="G27" t="s">
-        <v>429</v>
+        <v>364</v>
       </c>
       <c r="H27" t="s">
-        <v>430</v>
+        <v>365</v>
       </c>
       <c r="I27">
         <v>0</v>
@@ -5622,19 +5382,19 @@
         <v>25</v>
       </c>
       <c r="D28" t="s">
-        <v>226</v>
+        <v>186</v>
       </c>
       <c r="E28" t="s">
-        <v>227</v>
+        <v>187</v>
       </c>
       <c r="F28" t="s">
-        <v>228</v>
+        <v>188</v>
       </c>
       <c r="G28" t="s">
-        <v>229</v>
+        <v>189</v>
       </c>
       <c r="H28" t="s">
-        <v>230</v>
+        <v>190</v>
       </c>
       <c r="I28">
         <v>0</v>
@@ -5732,19 +5492,19 @@
         <v>25</v>
       </c>
       <c r="D29" t="s">
-        <v>356</v>
+        <v>301</v>
       </c>
       <c r="E29" t="s">
-        <v>357</v>
+        <v>302</v>
       </c>
       <c r="F29" t="s">
-        <v>358</v>
+        <v>303</v>
       </c>
       <c r="G29" t="s">
-        <v>359</v>
+        <v>304</v>
       </c>
       <c r="H29" t="s">
-        <v>360</v>
+        <v>305</v>
       </c>
       <c r="I29">
         <v>0</v>
@@ -5854,19 +5614,19 @@
         <v>25</v>
       </c>
       <c r="D30" t="s">
-        <v>296</v>
+        <v>251</v>
       </c>
       <c r="E30" t="s">
-        <v>297</v>
+        <v>252</v>
       </c>
       <c r="F30" t="s">
-        <v>298</v>
+        <v>253</v>
       </c>
       <c r="G30" t="s">
-        <v>299</v>
+        <v>254</v>
       </c>
       <c r="H30" t="s">
-        <v>300</v>
+        <v>255</v>
       </c>
       <c r="I30">
         <v>0</v>
@@ -5955,19 +5715,19 @@
         <v>25</v>
       </c>
       <c r="D31" t="s">
-        <v>631</v>
+        <v>556</v>
       </c>
       <c r="E31" t="s">
-        <v>632</v>
+        <v>557</v>
       </c>
       <c r="F31" t="s">
-        <v>633</v>
+        <v>558</v>
       </c>
       <c r="G31" t="s">
-        <v>634</v>
+        <v>559</v>
       </c>
       <c r="H31" t="s">
-        <v>635</v>
+        <v>560</v>
       </c>
       <c r="I31">
         <v>0</v>
@@ -6074,19 +5834,19 @@
         <v>25</v>
       </c>
       <c r="D32" t="s">
-        <v>336</v>
+        <v>286</v>
       </c>
       <c r="E32" t="s">
-        <v>337</v>
+        <v>287</v>
       </c>
       <c r="F32" t="s">
-        <v>338</v>
+        <v>288</v>
       </c>
       <c r="G32" t="s">
-        <v>339</v>
+        <v>289</v>
       </c>
       <c r="H32" t="s">
-        <v>340</v>
+        <v>290</v>
       </c>
       <c r="I32">
         <v>0</v>
@@ -6196,19 +5956,19 @@
         <v>25</v>
       </c>
       <c r="D33" t="s">
-        <v>216</v>
+        <v>176</v>
       </c>
       <c r="E33" t="s">
-        <v>217</v>
+        <v>177</v>
       </c>
       <c r="F33" t="s">
-        <v>218</v>
+        <v>178</v>
       </c>
       <c r="G33" t="s">
-        <v>219</v>
+        <v>179</v>
       </c>
       <c r="H33" t="s">
-        <v>220</v>
+        <v>180</v>
       </c>
       <c r="I33">
         <v>0</v>
@@ -6294,19 +6054,19 @@
         <v>25</v>
       </c>
       <c r="D34" t="s">
-        <v>46</v>
+        <v>41</v>
       </c>
       <c r="E34" t="s">
-        <v>47</v>
+        <v>42</v>
       </c>
       <c r="F34" t="s">
-        <v>48</v>
+        <v>43</v>
       </c>
       <c r="G34" t="s">
-        <v>49</v>
+        <v>44</v>
       </c>
       <c r="H34" t="s">
-        <v>50</v>
+        <v>45</v>
       </c>
       <c r="I34">
         <v>0</v>
@@ -6416,19 +6176,19 @@
         <v>25</v>
       </c>
       <c r="D35" t="s">
-        <v>576</v>
+        <v>501</v>
       </c>
       <c r="E35" t="s">
-        <v>577</v>
+        <v>502</v>
       </c>
       <c r="F35" t="s">
-        <v>578</v>
+        <v>503</v>
       </c>
       <c r="G35" t="s">
-        <v>579</v>
+        <v>504</v>
       </c>
       <c r="H35" t="s">
-        <v>580</v>
+        <v>505</v>
       </c>
       <c r="I35">
         <v>0</v>
@@ -6538,19 +6298,19 @@
         <v>25</v>
       </c>
       <c r="D36" t="s">
-        <v>71</v>
+        <v>61</v>
       </c>
       <c r="E36" t="s">
-        <v>72</v>
+        <v>62</v>
       </c>
       <c r="F36" t="s">
-        <v>73</v>
+        <v>63</v>
       </c>
       <c r="G36" t="s">
-        <v>74</v>
+        <v>64</v>
       </c>
       <c r="H36" t="s">
-        <v>75</v>
+        <v>65</v>
       </c>
       <c r="I36">
         <v>0</v>
@@ -6639,19 +6399,19 @@
         <v>25</v>
       </c>
       <c r="D37" t="s">
-        <v>366</v>
+        <v>311</v>
       </c>
       <c r="E37" t="s">
-        <v>367</v>
+        <v>312</v>
       </c>
       <c r="F37" t="s">
-        <v>368</v>
+        <v>313</v>
       </c>
       <c r="G37" t="s">
-        <v>369</v>
+        <v>314</v>
       </c>
       <c r="H37" t="s">
-        <v>370</v>
+        <v>315</v>
       </c>
       <c r="I37">
         <v>0</v>
@@ -6761,19 +6521,19 @@
         <v>25</v>
       </c>
       <c r="D38" t="s">
-        <v>571</v>
+        <v>496</v>
       </c>
       <c r="E38" t="s">
-        <v>572</v>
+        <v>497</v>
       </c>
       <c r="F38" t="s">
-        <v>573</v>
+        <v>498</v>
       </c>
       <c r="G38" t="s">
-        <v>574</v>
+        <v>499</v>
       </c>
       <c r="H38" t="s">
-        <v>575</v>
+        <v>500</v>
       </c>
       <c r="I38">
         <v>0</v>
@@ -6877,19 +6637,19 @@
         <v>25</v>
       </c>
       <c r="D39" t="s">
-        <v>601</v>
+        <v>526</v>
       </c>
       <c r="E39" t="s">
-        <v>602</v>
+        <v>527</v>
       </c>
       <c r="F39" t="s">
-        <v>603</v>
+        <v>528</v>
       </c>
       <c r="G39" t="s">
-        <v>604</v>
+        <v>529</v>
       </c>
       <c r="H39" t="s">
-        <v>605</v>
+        <v>530</v>
       </c>
       <c r="I39">
         <v>0</v>
@@ -6999,19 +6759,19 @@
         <v>25</v>
       </c>
       <c r="D40" t="s">
-        <v>551</v>
+        <v>476</v>
       </c>
       <c r="E40" t="s">
-        <v>552</v>
+        <v>477</v>
       </c>
       <c r="F40" t="s">
-        <v>553</v>
+        <v>478</v>
       </c>
       <c r="G40" t="s">
-        <v>554</v>
+        <v>479</v>
       </c>
       <c r="H40" t="s">
-        <v>555</v>
+        <v>480</v>
       </c>
       <c r="I40">
         <v>0</v>
@@ -7109,19 +6869,19 @@
         <v>25</v>
       </c>
       <c r="D41" t="s">
-        <v>406</v>
+        <v>351</v>
       </c>
       <c r="E41" t="s">
-        <v>407</v>
+        <v>352</v>
       </c>
       <c r="F41" t="s">
-        <v>408</v>
+        <v>353</v>
       </c>
       <c r="G41" t="s">
-        <v>409</v>
+        <v>354</v>
       </c>
       <c r="H41" t="s">
-        <v>410</v>
+        <v>355</v>
       </c>
       <c r="I41">
         <v>0</v>
@@ -7231,19 +6991,19 @@
         <v>25</v>
       </c>
       <c r="D42" t="s">
-        <v>446</v>
+        <v>376</v>
       </c>
       <c r="E42" t="s">
-        <v>447</v>
+        <v>377</v>
       </c>
       <c r="F42" t="s">
-        <v>448</v>
+        <v>378</v>
       </c>
       <c r="G42" t="s">
-        <v>449</v>
+        <v>379</v>
       </c>
       <c r="H42" t="s">
-        <v>450</v>
+        <v>380</v>
       </c>
       <c r="I42">
         <v>0</v>
@@ -7353,19 +7113,19 @@
         <v>25</v>
       </c>
       <c r="D43" t="s">
-        <v>626</v>
+        <v>551</v>
       </c>
       <c r="E43" t="s">
-        <v>627</v>
+        <v>552</v>
       </c>
       <c r="F43" t="s">
-        <v>628</v>
+        <v>553</v>
       </c>
       <c r="G43" t="s">
-        <v>629</v>
+        <v>554</v>
       </c>
       <c r="H43" t="s">
-        <v>630</v>
+        <v>555</v>
       </c>
       <c r="I43">
         <v>0</v>
@@ -7469,19 +7229,19 @@
         <v>25</v>
       </c>
       <c r="D44" t="s">
-        <v>116</v>
+        <v>91</v>
       </c>
       <c r="E44" t="s">
-        <v>117</v>
+        <v>92</v>
       </c>
       <c r="F44" t="s">
-        <v>118</v>
+        <v>93</v>
       </c>
       <c r="G44" t="s">
-        <v>119</v>
+        <v>94</v>
       </c>
       <c r="H44" t="s">
-        <v>120</v>
+        <v>95</v>
       </c>
       <c r="I44">
         <v>0</v>
@@ -7591,19 +7351,19 @@
         <v>25</v>
       </c>
       <c r="D45" t="s">
-        <v>151</v>
+        <v>121</v>
       </c>
       <c r="E45" t="s">
-        <v>152</v>
+        <v>122</v>
       </c>
       <c r="F45" t="s">
-        <v>153</v>
+        <v>123</v>
       </c>
       <c r="G45" t="s">
-        <v>154</v>
+        <v>124</v>
       </c>
       <c r="H45" t="s">
-        <v>155</v>
+        <v>125</v>
       </c>
       <c r="I45">
         <v>0</v>
@@ -7713,19 +7473,19 @@
         <v>25</v>
       </c>
       <c r="D46" t="s">
-        <v>391</v>
+        <v>336</v>
       </c>
       <c r="E46" t="s">
-        <v>392</v>
+        <v>337</v>
       </c>
       <c r="F46" t="s">
-        <v>393</v>
+        <v>338</v>
       </c>
       <c r="G46" t="s">
-        <v>394</v>
+        <v>339</v>
       </c>
       <c r="H46" t="s">
-        <v>395</v>
+        <v>340</v>
       </c>
       <c r="I46">
         <v>0</v>
@@ -7811,19 +7571,19 @@
         <v>25</v>
       </c>
       <c r="D47" t="s">
-        <v>276</v>
+        <v>236</v>
       </c>
       <c r="E47" t="s">
-        <v>277</v>
+        <v>237</v>
       </c>
       <c r="F47" t="s">
-        <v>278</v>
+        <v>238</v>
       </c>
       <c r="G47" t="s">
-        <v>279</v>
+        <v>239</v>
       </c>
       <c r="H47" t="s">
-        <v>280</v>
+        <v>240</v>
       </c>
       <c r="I47">
         <v>0</v>
@@ -7933,19 +7693,19 @@
         <v>25</v>
       </c>
       <c r="D48" t="s">
-        <v>546</v>
+        <v>471</v>
       </c>
       <c r="E48" t="s">
-        <v>547</v>
+        <v>472</v>
       </c>
       <c r="F48" t="s">
-        <v>548</v>
+        <v>473</v>
       </c>
       <c r="G48" t="s">
-        <v>549</v>
+        <v>474</v>
       </c>
       <c r="H48" t="s">
-        <v>550</v>
+        <v>475</v>
       </c>
       <c r="I48">
         <v>0</v>
@@ -8055,19 +7815,19 @@
         <v>25</v>
       </c>
       <c r="D49" t="s">
-        <v>326</v>
+        <v>276</v>
       </c>
       <c r="E49" t="s">
-        <v>327</v>
+        <v>277</v>
       </c>
       <c r="F49" t="s">
-        <v>328</v>
+        <v>278</v>
       </c>
       <c r="G49" t="s">
-        <v>329</v>
+        <v>279</v>
       </c>
       <c r="H49" t="s">
-        <v>330</v>
+        <v>280</v>
       </c>
       <c r="I49">
         <v>0</v>
@@ -8165,19 +7925,19 @@
         <v>25</v>
       </c>
       <c r="D50" t="s">
-        <v>386</v>
+        <v>331</v>
       </c>
       <c r="E50" t="s">
-        <v>387</v>
+        <v>332</v>
       </c>
       <c r="F50" t="s">
-        <v>388</v>
+        <v>333</v>
       </c>
       <c r="G50" t="s">
-        <v>389</v>
+        <v>334</v>
       </c>
       <c r="H50" t="s">
-        <v>390</v>
+        <v>335</v>
       </c>
       <c r="I50">
         <v>0</v>
@@ -8287,19 +8047,19 @@
         <v>25</v>
       </c>
       <c r="D51" t="s">
-        <v>521</v>
+        <v>451</v>
       </c>
       <c r="E51" t="s">
-        <v>522</v>
+        <v>452</v>
       </c>
       <c r="F51" t="s">
-        <v>523</v>
+        <v>453</v>
       </c>
       <c r="G51" t="s">
-        <v>524</v>
+        <v>454</v>
       </c>
       <c r="H51" t="s">
-        <v>525</v>
+        <v>455</v>
       </c>
       <c r="I51">
         <v>0</v>
@@ -8406,19 +8166,19 @@
         <v>25</v>
       </c>
       <c r="D52" t="s">
-        <v>401</v>
+        <v>346</v>
       </c>
       <c r="E52" t="s">
-        <v>402</v>
+        <v>347</v>
       </c>
       <c r="F52" t="s">
-        <v>403</v>
+        <v>348</v>
       </c>
       <c r="G52" t="s">
-        <v>404</v>
+        <v>349</v>
       </c>
       <c r="H52" t="s">
-        <v>405</v>
+        <v>350</v>
       </c>
       <c r="I52">
         <v>0</v>
@@ -8510,19 +8270,19 @@
         <v>25</v>
       </c>
       <c r="D53" t="s">
-        <v>396</v>
+        <v>341</v>
       </c>
       <c r="E53" t="s">
-        <v>397</v>
+        <v>342</v>
       </c>
       <c r="F53" t="s">
-        <v>398</v>
+        <v>343</v>
       </c>
       <c r="G53" t="s">
-        <v>399</v>
+        <v>344</v>
       </c>
       <c r="H53" t="s">
-        <v>400</v>
+        <v>345</v>
       </c>
       <c r="I53">
         <v>0</v>
@@ -8632,19 +8392,19 @@
         <v>25</v>
       </c>
       <c r="D54" t="s">
-        <v>581</v>
+        <v>506</v>
       </c>
       <c r="E54" t="s">
-        <v>582</v>
+        <v>507</v>
       </c>
       <c r="F54" t="s">
-        <v>583</v>
+        <v>508</v>
       </c>
       <c r="G54" t="s">
-        <v>584</v>
+        <v>509</v>
       </c>
       <c r="H54" t="s">
-        <v>585</v>
+        <v>510</v>
       </c>
       <c r="I54">
         <v>0</v>
@@ -8754,19 +8514,19 @@
         <v>25</v>
       </c>
       <c r="D55" t="s">
-        <v>281</v>
+        <v>241</v>
       </c>
       <c r="E55" t="s">
-        <v>282</v>
+        <v>242</v>
       </c>
       <c r="F55" t="s">
-        <v>283</v>
+        <v>243</v>
       </c>
       <c r="G55" t="s">
-        <v>284</v>
+        <v>244</v>
       </c>
       <c r="H55" t="s">
-        <v>285</v>
+        <v>245</v>
       </c>
       <c r="I55">
         <v>0</v>
@@ -8876,19 +8636,19 @@
         <v>25</v>
       </c>
       <c r="D56" t="s">
-        <v>451</v>
+        <v>381</v>
       </c>
       <c r="E56" t="s">
-        <v>452</v>
+        <v>382</v>
       </c>
       <c r="F56" t="s">
-        <v>453</v>
+        <v>383</v>
       </c>
       <c r="G56" t="s">
-        <v>454</v>
+        <v>384</v>
       </c>
       <c r="H56" t="s">
-        <v>455</v>
+        <v>385</v>
       </c>
       <c r="I56">
         <v>0</v>
@@ -8998,19 +8758,19 @@
         <v>25</v>
       </c>
       <c r="D57" t="s">
-        <v>466</v>
+        <v>396</v>
       </c>
       <c r="E57" t="s">
-        <v>467</v>
+        <v>397</v>
       </c>
       <c r="F57" t="s">
-        <v>468</v>
+        <v>398</v>
       </c>
       <c r="G57" t="s">
-        <v>469</v>
+        <v>399</v>
       </c>
       <c r="H57" t="s">
-        <v>470</v>
+        <v>400</v>
       </c>
       <c r="I57">
         <v>0</v>
@@ -9120,19 +8880,19 @@
         <v>25</v>
       </c>
       <c r="D58" t="s">
-        <v>561</v>
+        <v>486</v>
       </c>
       <c r="E58" t="s">
-        <v>562</v>
+        <v>487</v>
       </c>
       <c r="F58" t="s">
-        <v>563</v>
+        <v>488</v>
       </c>
       <c r="G58" t="s">
-        <v>564</v>
+        <v>489</v>
       </c>
       <c r="H58" t="s">
-        <v>565</v>
+        <v>490</v>
       </c>
       <c r="I58">
         <v>0</v>
@@ -9242,19 +9002,19 @@
         <v>25</v>
       </c>
       <c r="D59" t="s">
-        <v>286</v>
+        <v>246</v>
       </c>
       <c r="E59" t="s">
-        <v>287</v>
+        <v>247</v>
       </c>
       <c r="F59" t="s">
-        <v>288</v>
+        <v>248</v>
       </c>
       <c r="G59" t="s">
-        <v>289</v>
+        <v>249</v>
       </c>
       <c r="H59" t="s">
-        <v>290</v>
+        <v>250</v>
       </c>
       <c r="I59">
         <v>0</v>
@@ -9364,19 +9124,19 @@
         <v>25</v>
       </c>
       <c r="D60" t="s">
-        <v>171</v>
+        <v>136</v>
       </c>
       <c r="E60" t="s">
-        <v>172</v>
+        <v>137</v>
       </c>
       <c r="F60" t="s">
-        <v>173</v>
+        <v>138</v>
       </c>
       <c r="G60" t="s">
-        <v>174</v>
+        <v>139</v>
       </c>
       <c r="H60" t="s">
-        <v>175</v>
+        <v>140</v>
       </c>
       <c r="I60">
         <v>0</v>
@@ -9486,19 +9246,19 @@
         <v>25</v>
       </c>
       <c r="D61" t="s">
-        <v>476</v>
+        <v>406</v>
       </c>
       <c r="E61" t="s">
-        <v>477</v>
+        <v>407</v>
       </c>
       <c r="F61" t="s">
-        <v>478</v>
+        <v>408</v>
       </c>
       <c r="G61" t="s">
-        <v>479</v>
+        <v>409</v>
       </c>
       <c r="H61" t="s">
-        <v>480</v>
+        <v>410</v>
       </c>
       <c r="I61">
         <v>0</v>
@@ -9602,19 +9362,19 @@
         <v>25</v>
       </c>
       <c r="D62" t="s">
-        <v>436</v>
+        <v>371</v>
       </c>
       <c r="E62" t="s">
-        <v>437</v>
+        <v>372</v>
       </c>
       <c r="F62" t="s">
-        <v>438</v>
+        <v>373</v>
       </c>
       <c r="G62" t="s">
-        <v>439</v>
+        <v>374</v>
       </c>
       <c r="H62" t="s">
-        <v>440</v>
+        <v>375</v>
       </c>
       <c r="I62">
         <v>0</v>
@@ -9724,19 +9484,19 @@
         <v>25</v>
       </c>
       <c r="D63" t="s">
-        <v>81</v>
+        <v>71</v>
       </c>
       <c r="E63" t="s">
-        <v>82</v>
+        <v>72</v>
       </c>
       <c r="F63" t="s">
-        <v>83</v>
+        <v>73</v>
       </c>
       <c r="G63" t="s">
-        <v>84</v>
+        <v>74</v>
       </c>
       <c r="H63" t="s">
-        <v>85</v>
+        <v>75</v>
       </c>
       <c r="I63">
         <v>0</v>
@@ -9843,19 +9603,19 @@
         <v>25</v>
       </c>
       <c r="D64" t="s">
-        <v>136</v>
+        <v>111</v>
       </c>
       <c r="E64" t="s">
-        <v>137</v>
+        <v>112</v>
       </c>
       <c r="F64" t="s">
-        <v>138</v>
+        <v>113</v>
       </c>
       <c r="G64" t="s">
-        <v>139</v>
+        <v>114</v>
       </c>
       <c r="H64" t="s">
-        <v>140</v>
+        <v>115</v>
       </c>
       <c r="I64">
         <v>0</v>
@@ -9947,19 +9707,19 @@
         <v>25</v>
       </c>
       <c r="D65" t="s">
-        <v>596</v>
+        <v>521</v>
       </c>
       <c r="E65" t="s">
-        <v>597</v>
+        <v>522</v>
       </c>
       <c r="F65" t="s">
-        <v>598</v>
+        <v>523</v>
       </c>
       <c r="G65" t="s">
-        <v>599</v>
+        <v>524</v>
       </c>
       <c r="H65" t="s">
-        <v>600</v>
+        <v>525</v>
       </c>
       <c r="I65">
         <v>0</v>
@@ -10054,19 +9814,19 @@
         <v>25</v>
       </c>
       <c r="D66" t="s">
-        <v>321</v>
+        <v>271</v>
       </c>
       <c r="E66" t="s">
-        <v>322</v>
+        <v>272</v>
       </c>
       <c r="F66" t="s">
-        <v>323</v>
+        <v>273</v>
       </c>
       <c r="G66" t="s">
-        <v>324</v>
+        <v>274</v>
       </c>
       <c r="H66" t="s">
-        <v>325</v>
+        <v>275</v>
       </c>
       <c r="I66">
         <v>0</v>
@@ -10158,19 +9918,19 @@
         <v>25</v>
       </c>
       <c r="D67" t="s">
-        <v>236</v>
+        <v>196</v>
       </c>
       <c r="E67" t="s">
-        <v>237</v>
+        <v>197</v>
       </c>
       <c r="F67" t="s">
-        <v>238</v>
+        <v>198</v>
       </c>
       <c r="G67" t="s">
-        <v>239</v>
+        <v>199</v>
       </c>
       <c r="H67" t="s">
-        <v>240</v>
+        <v>200</v>
       </c>
       <c r="I67">
         <v>0</v>
@@ -10280,19 +10040,19 @@
         <v>25</v>
       </c>
       <c r="D68" t="s">
-        <v>186</v>
+        <v>146</v>
       </c>
       <c r="E68" t="s">
-        <v>187</v>
+        <v>147</v>
       </c>
       <c r="F68" t="s">
-        <v>188</v>
+        <v>148</v>
       </c>
       <c r="G68" t="s">
-        <v>189</v>
+        <v>149</v>
       </c>
       <c r="H68" t="s">
-        <v>190</v>
+        <v>150</v>
       </c>
       <c r="I68">
         <v>0</v>
@@ -10402,19 +10162,19 @@
         <v>25</v>
       </c>
       <c r="D69" t="s">
-        <v>531</v>
+        <v>461</v>
       </c>
       <c r="E69" t="s">
-        <v>532</v>
+        <v>462</v>
       </c>
       <c r="F69" t="s">
-        <v>533</v>
+        <v>463</v>
       </c>
       <c r="G69" t="s">
-        <v>534</v>
+        <v>464</v>
       </c>
       <c r="H69" t="s">
-        <v>535</v>
+        <v>465</v>
       </c>
       <c r="I69">
         <v>0</v>
@@ -10524,19 +10284,19 @@
         <v>25</v>
       </c>
       <c r="D70" t="s">
-        <v>181</v>
+        <v>141</v>
       </c>
       <c r="E70" t="s">
-        <v>182</v>
+        <v>142</v>
       </c>
       <c r="F70" t="s">
-        <v>183</v>
+        <v>143</v>
       </c>
       <c r="G70" t="s">
-        <v>184</v>
+        <v>144</v>
       </c>
       <c r="H70" t="s">
-        <v>185</v>
+        <v>145</v>
       </c>
       <c r="I70">
         <v>0</v>
@@ -10646,19 +10406,19 @@
         <v>25</v>
       </c>
       <c r="D71" t="s">
-        <v>411</v>
+        <v>356</v>
       </c>
       <c r="E71" t="s">
-        <v>412</v>
+        <v>357</v>
       </c>
       <c r="F71" t="s">
-        <v>413</v>
+        <v>358</v>
       </c>
       <c r="G71" t="s">
-        <v>414</v>
+        <v>359</v>
       </c>
       <c r="H71" t="s">
-        <v>415</v>
+        <v>360</v>
       </c>
       <c r="I71">
         <v>0</v>
@@ -10765,19 +10525,19 @@
         <v>25</v>
       </c>
       <c r="D72" t="s">
-        <v>256</v>
+        <v>216</v>
       </c>
       <c r="E72" t="s">
-        <v>257</v>
+        <v>217</v>
       </c>
       <c r="F72" t="s">
-        <v>258</v>
+        <v>218</v>
       </c>
       <c r="G72" t="s">
-        <v>259</v>
+        <v>219</v>
       </c>
       <c r="H72" t="s">
-        <v>260</v>
+        <v>220</v>
       </c>
       <c r="I72">
         <v>0</v>
@@ -10887,19 +10647,19 @@
         <v>25</v>
       </c>
       <c r="D73" t="s">
-        <v>486</v>
+        <v>416</v>
       </c>
       <c r="E73" t="s">
-        <v>487</v>
+        <v>417</v>
       </c>
       <c r="F73" t="s">
-        <v>488</v>
+        <v>418</v>
       </c>
       <c r="G73" t="s">
-        <v>489</v>
+        <v>419</v>
       </c>
       <c r="H73" t="s">
-        <v>490</v>
+        <v>420</v>
       </c>
       <c r="I73">
         <v>0</v>
@@ -10991,19 +10751,19 @@
         <v>25</v>
       </c>
       <c r="D74" t="s">
-        <v>351</v>
+        <v>296</v>
       </c>
       <c r="E74" t="s">
-        <v>352</v>
+        <v>297</v>
       </c>
       <c r="F74" t="s">
-        <v>353</v>
+        <v>298</v>
       </c>
       <c r="G74" t="s">
-        <v>354</v>
+        <v>299</v>
       </c>
       <c r="H74" t="s">
-        <v>355</v>
+        <v>300</v>
       </c>
       <c r="I74">
         <v>0</v>
@@ -11113,19 +10873,19 @@
         <v>25</v>
       </c>
       <c r="D75" t="s">
-        <v>201</v>
+        <v>161</v>
       </c>
       <c r="E75" t="s">
-        <v>202</v>
+        <v>162</v>
       </c>
       <c r="F75" t="s">
-        <v>203</v>
+        <v>163</v>
       </c>
       <c r="G75" t="s">
-        <v>204</v>
+        <v>164</v>
       </c>
       <c r="H75" t="s">
-        <v>205</v>
+        <v>165</v>
       </c>
       <c r="I75">
         <v>0</v>
@@ -11235,19 +10995,19 @@
         <v>25</v>
       </c>
       <c r="D76" t="s">
-        <v>376</v>
+        <v>321</v>
       </c>
       <c r="E76" t="s">
-        <v>377</v>
+        <v>322</v>
       </c>
       <c r="F76" t="s">
-        <v>378</v>
+        <v>323</v>
       </c>
       <c r="G76" t="s">
-        <v>379</v>
+        <v>324</v>
       </c>
       <c r="H76" t="s">
-        <v>380</v>
+        <v>325</v>
       </c>
       <c r="I76">
         <v>0</v>
@@ -11357,19 +11117,19 @@
         <v>25</v>
       </c>
       <c r="D77" t="s">
-        <v>586</v>
+        <v>511</v>
       </c>
       <c r="E77" t="s">
-        <v>587</v>
+        <v>512</v>
       </c>
       <c r="F77" t="s">
-        <v>588</v>
+        <v>513</v>
       </c>
       <c r="G77" t="s">
-        <v>589</v>
+        <v>514</v>
       </c>
       <c r="H77" t="s">
-        <v>590</v>
+        <v>515</v>
       </c>
       <c r="I77">
         <v>0</v>
@@ -11479,19 +11239,19 @@
         <v>25</v>
       </c>
       <c r="D78" t="s">
-        <v>491</v>
+        <v>421</v>
       </c>
       <c r="E78" t="s">
-        <v>492</v>
+        <v>422</v>
       </c>
       <c r="F78" t="s">
-        <v>493</v>
+        <v>423</v>
       </c>
       <c r="G78" t="s">
-        <v>494</v>
+        <v>424</v>
       </c>
       <c r="H78" t="s">
-        <v>495</v>
+        <v>425</v>
       </c>
       <c r="I78">
         <v>0</v>
@@ -11592,19 +11352,19 @@
         <v>25</v>
       </c>
       <c r="D79" t="s">
-        <v>641</v>
+        <v>561</v>
       </c>
       <c r="E79" t="s">
-        <v>642</v>
+        <v>562</v>
       </c>
       <c r="F79" t="s">
-        <v>643</v>
+        <v>563</v>
       </c>
       <c r="G79" t="s">
-        <v>644</v>
+        <v>564</v>
       </c>
       <c r="H79" t="s">
-        <v>645</v>
+        <v>565</v>
       </c>
       <c r="I79">
         <v>0</v>
@@ -11711,19 +11471,19 @@
         <v>25</v>
       </c>
       <c r="D80" t="s">
-        <v>191</v>
+        <v>151</v>
       </c>
       <c r="E80" t="s">
-        <v>192</v>
+        <v>152</v>
       </c>
       <c r="F80" t="s">
-        <v>193</v>
+        <v>153</v>
       </c>
       <c r="G80" t="s">
-        <v>194</v>
+        <v>154</v>
       </c>
       <c r="H80" t="s">
-        <v>195</v>
+        <v>155</v>
       </c>
       <c r="I80">
         <v>0</v>
@@ -11833,19 +11593,19 @@
         <v>25</v>
       </c>
       <c r="D81" t="s">
-        <v>556</v>
+        <v>481</v>
       </c>
       <c r="E81" t="s">
-        <v>557</v>
+        <v>482</v>
       </c>
       <c r="F81" t="s">
-        <v>558</v>
+        <v>483</v>
       </c>
       <c r="G81" t="s">
-        <v>559</v>
+        <v>484</v>
       </c>
       <c r="H81" t="s">
-        <v>560</v>
+        <v>485</v>
       </c>
       <c r="I81">
         <v>0</v>
@@ -11955,19 +11715,19 @@
         <v>25</v>
       </c>
       <c r="D82" t="s">
-        <v>196</v>
+        <v>156</v>
       </c>
       <c r="E82" t="s">
-        <v>197</v>
+        <v>157</v>
       </c>
       <c r="F82" t="s">
-        <v>198</v>
+        <v>158</v>
       </c>
       <c r="G82" t="s">
-        <v>199</v>
+        <v>159</v>
       </c>
       <c r="H82" t="s">
-        <v>200</v>
+        <v>160</v>
       </c>
       <c r="I82">
         <v>0</v>
@@ -12077,19 +11837,19 @@
         <v>25</v>
       </c>
       <c r="D83" t="s">
-        <v>526</v>
+        <v>456</v>
       </c>
       <c r="E83" t="s">
-        <v>527</v>
+        <v>457</v>
       </c>
       <c r="F83" t="s">
-        <v>528</v>
+        <v>458</v>
       </c>
       <c r="G83" t="s">
-        <v>529</v>
+        <v>459</v>
       </c>
       <c r="H83" t="s">
-        <v>530</v>
+        <v>460</v>
       </c>
       <c r="I83">
         <v>0</v>
@@ -12199,19 +11959,19 @@
         <v>25</v>
       </c>
       <c r="D84" t="s">
-        <v>76</v>
+        <v>66</v>
       </c>
       <c r="E84" t="s">
-        <v>77</v>
+        <v>67</v>
       </c>
       <c r="F84" t="s">
-        <v>78</v>
+        <v>68</v>
       </c>
       <c r="G84" t="s">
-        <v>79</v>
+        <v>69</v>
       </c>
       <c r="H84" t="s">
-        <v>80</v>
+        <v>70</v>
       </c>
       <c r="I84">
         <v>0</v>
@@ -12294,19 +12054,19 @@
         <v>25</v>
       </c>
       <c r="D85" t="s">
-        <v>241</v>
+        <v>201</v>
       </c>
       <c r="E85" t="s">
-        <v>242</v>
+        <v>202</v>
       </c>
       <c r="F85" t="s">
-        <v>243</v>
+        <v>203</v>
       </c>
       <c r="G85" t="s">
-        <v>244</v>
+        <v>204</v>
       </c>
       <c r="H85" t="s">
-        <v>245</v>
+        <v>205</v>
       </c>
       <c r="I85">
         <v>0</v>
@@ -12416,19 +12176,19 @@
         <v>25</v>
       </c>
       <c r="D86" t="s">
-        <v>266</v>
+        <v>226</v>
       </c>
       <c r="E86" t="s">
-        <v>267</v>
+        <v>227</v>
       </c>
       <c r="F86" t="s">
-        <v>268</v>
+        <v>228</v>
       </c>
       <c r="G86" t="s">
-        <v>269</v>
+        <v>229</v>
       </c>
       <c r="H86" t="s">
-        <v>270</v>
+        <v>230</v>
       </c>
       <c r="I86">
         <v>0</v>
@@ -12538,19 +12298,19 @@
         <v>25</v>
       </c>
       <c r="D87" t="s">
-        <v>271</v>
+        <v>231</v>
       </c>
       <c r="E87" t="s">
-        <v>272</v>
+        <v>232</v>
       </c>
       <c r="F87" t="s">
-        <v>273</v>
+        <v>233</v>
       </c>
       <c r="G87" t="s">
-        <v>274</v>
+        <v>234</v>
       </c>
       <c r="H87" t="s">
-        <v>275</v>
+        <v>235</v>
       </c>
       <c r="I87">
         <v>0</v>
@@ -12660,19 +12420,19 @@
         <v>25</v>
       </c>
       <c r="D88" t="s">
-        <v>126</v>
+        <v>101</v>
       </c>
       <c r="E88" t="s">
-        <v>127</v>
+        <v>102</v>
       </c>
       <c r="F88" t="s">
-        <v>128</v>
+        <v>103</v>
       </c>
       <c r="G88" t="s">
-        <v>129</v>
+        <v>104</v>
       </c>
       <c r="H88" t="s">
-        <v>130</v>
+        <v>105</v>
       </c>
       <c r="I88">
         <v>0</v>
@@ -12782,19 +12542,19 @@
         <v>25</v>
       </c>
       <c r="D89" t="s">
-        <v>606</v>
+        <v>531</v>
       </c>
       <c r="E89" t="s">
-        <v>607</v>
+        <v>532</v>
       </c>
       <c r="F89" t="s">
-        <v>608</v>
+        <v>533</v>
       </c>
       <c r="G89" t="s">
-        <v>609</v>
+        <v>534</v>
       </c>
       <c r="H89" t="s">
-        <v>610</v>
+        <v>535</v>
       </c>
       <c r="I89">
         <v>0</v>
@@ -12904,19 +12664,19 @@
         <v>25</v>
       </c>
       <c r="D90" t="s">
-        <v>381</v>
+        <v>326</v>
       </c>
       <c r="E90" t="s">
-        <v>382</v>
+        <v>327</v>
       </c>
       <c r="F90" t="s">
-        <v>383</v>
+        <v>328</v>
       </c>
       <c r="G90" t="s">
-        <v>384</v>
+        <v>329</v>
       </c>
       <c r="H90" t="s">
-        <v>385</v>
+        <v>330</v>
       </c>
       <c r="I90">
         <v>0</v>
@@ -13026,19 +12786,19 @@
         <v>25</v>
       </c>
       <c r="D91" t="s">
-        <v>496</v>
+        <v>426</v>
       </c>
       <c r="E91" t="s">
-        <v>497</v>
+        <v>427</v>
       </c>
       <c r="F91" t="s">
-        <v>498</v>
+        <v>428</v>
       </c>
       <c r="G91" t="s">
-        <v>499</v>
+        <v>429</v>
       </c>
       <c r="H91" t="s">
-        <v>500</v>
+        <v>430</v>
       </c>
       <c r="I91">
         <v>0</v>
@@ -13148,19 +12908,19 @@
         <v>25</v>
       </c>
       <c r="D92" t="s">
-        <v>456</v>
+        <v>386</v>
       </c>
       <c r="E92" t="s">
-        <v>457</v>
+        <v>387</v>
       </c>
       <c r="F92" t="s">
-        <v>458</v>
+        <v>388</v>
       </c>
       <c r="G92" t="s">
-        <v>459</v>
+        <v>389</v>
       </c>
       <c r="H92" t="s">
-        <v>460</v>
+        <v>390</v>
       </c>
       <c r="I92">
         <v>0</v>
@@ -13264,19 +13024,19 @@
         <v>25</v>
       </c>
       <c r="D93" t="s">
-        <v>66</v>
+        <v>56</v>
       </c>
       <c r="E93" t="s">
-        <v>67</v>
+        <v>57</v>
       </c>
       <c r="F93" t="s">
-        <v>68</v>
+        <v>58</v>
       </c>
       <c r="G93" t="s">
-        <v>69</v>
+        <v>59</v>
       </c>
       <c r="H93" t="s">
-        <v>70</v>
+        <v>60</v>
       </c>
       <c r="I93">
         <v>0</v>
@@ -13386,19 +13146,19 @@
         <v>25</v>
       </c>
       <c r="D94" t="s">
-        <v>156</v>
+        <v>126</v>
       </c>
       <c r="E94" t="s">
-        <v>157</v>
+        <v>127</v>
       </c>
       <c r="F94" t="s">
-        <v>158</v>
+        <v>128</v>
       </c>
       <c r="G94" t="s">
-        <v>159</v>
+        <v>129</v>
       </c>
       <c r="H94" t="s">
-        <v>160</v>
+        <v>130</v>
       </c>
       <c r="I94">
         <v>0</v>
@@ -13502,19 +13262,19 @@
         <v>25</v>
       </c>
       <c r="D95" t="s">
-        <v>361</v>
+        <v>306</v>
       </c>
       <c r="E95" t="s">
-        <v>362</v>
+        <v>307</v>
       </c>
       <c r="F95" t="s">
-        <v>363</v>
+        <v>308</v>
       </c>
       <c r="G95" t="s">
-        <v>364</v>
+        <v>309</v>
       </c>
       <c r="H95" t="s">
-        <v>365</v>
+        <v>310</v>
       </c>
       <c r="I95">
         <v>0</v>
@@ -13746,19 +13506,19 @@
         <v>25</v>
       </c>
       <c r="D97" t="s">
-        <v>161</v>
+        <v>131</v>
       </c>
       <c r="E97" t="s">
-        <v>162</v>
+        <v>132</v>
       </c>
       <c r="F97" t="s">
-        <v>163</v>
+        <v>133</v>
       </c>
       <c r="G97" t="s">
-        <v>164</v>
+        <v>134</v>
       </c>
       <c r="H97" t="s">
-        <v>165</v>
+        <v>135</v>
       </c>
       <c r="I97">
         <v>0</v>
@@ -13868,19 +13628,19 @@
         <v>25</v>
       </c>
       <c r="D98" t="s">
-        <v>51</v>
+        <v>46</v>
       </c>
       <c r="E98" t="s">
-        <v>52</v>
+        <v>47</v>
       </c>
       <c r="F98" t="s">
-        <v>53</v>
+        <v>48</v>
       </c>
       <c r="G98" t="s">
-        <v>54</v>
+        <v>49</v>
       </c>
       <c r="H98" t="s">
-        <v>55</v>
+        <v>50</v>
       </c>
       <c r="I98">
         <v>0</v>
@@ -13990,19 +13750,19 @@
         <v>25</v>
       </c>
       <c r="D99" t="s">
-        <v>371</v>
+        <v>316</v>
       </c>
       <c r="E99" t="s">
-        <v>372</v>
+        <v>317</v>
       </c>
       <c r="F99" t="s">
-        <v>373</v>
+        <v>318</v>
       </c>
       <c r="G99" t="s">
-        <v>374</v>
+        <v>319</v>
       </c>
       <c r="H99" t="s">
-        <v>375</v>
+        <v>320</v>
       </c>
       <c r="I99">
         <v>0</v>
@@ -14112,19 +13872,19 @@
         <v>25</v>
       </c>
       <c r="D100" t="s">
-        <v>121</v>
+        <v>96</v>
       </c>
       <c r="E100" t="s">
-        <v>122</v>
+        <v>97</v>
       </c>
       <c r="F100" t="s">
-        <v>123</v>
+        <v>98</v>
       </c>
       <c r="G100" t="s">
-        <v>124</v>
+        <v>99</v>
       </c>
       <c r="H100" t="s">
-        <v>125</v>
+        <v>100</v>
       </c>
       <c r="I100">
         <v>0</v>
@@ -14234,19 +13994,19 @@
         <v>25</v>
       </c>
       <c r="D101" t="s">
-        <v>481</v>
+        <v>411</v>
       </c>
       <c r="E101" t="s">
-        <v>482</v>
+        <v>412</v>
       </c>
       <c r="F101" t="s">
-        <v>483</v>
+        <v>413</v>
       </c>
       <c r="G101" t="s">
-        <v>484</v>
+        <v>414</v>
       </c>
       <c r="H101" t="s">
-        <v>485</v>
+        <v>415</v>
       </c>
       <c r="I101">
         <v>0</v>
@@ -14353,19 +14113,19 @@
         <v>25</v>
       </c>
       <c r="D102" t="s">
-        <v>131</v>
+        <v>106</v>
       </c>
       <c r="E102" t="s">
-        <v>132</v>
+        <v>107</v>
       </c>
       <c r="F102" t="s">
-        <v>133</v>
+        <v>108</v>
       </c>
       <c r="G102" t="s">
-        <v>134</v>
+        <v>109</v>
       </c>
       <c r="H102" t="s">
-        <v>135</v>
+        <v>110</v>
       </c>
       <c r="I102">
         <v>0</v>
@@ -14475,19 +14235,19 @@
         <v>25</v>
       </c>
       <c r="D103" t="s">
-        <v>61</v>
+        <v>51</v>
       </c>
       <c r="E103" t="s">
-        <v>62</v>
+        <v>52</v>
       </c>
       <c r="F103" t="s">
-        <v>63</v>
+        <v>53</v>
       </c>
       <c r="G103" t="s">
-        <v>64</v>
+        <v>54</v>
       </c>
       <c r="H103" t="s">
-        <v>65</v>
+        <v>55</v>
       </c>
       <c r="I103">
         <v>0</v>
@@ -14594,19 +14354,19 @@
         <v>25</v>
       </c>
       <c r="D104" t="s">
-        <v>251</v>
+        <v>211</v>
       </c>
       <c r="E104" t="s">
-        <v>252</v>
+        <v>212</v>
       </c>
       <c r="F104" t="s">
-        <v>253</v>
+        <v>213</v>
       </c>
       <c r="G104" t="s">
-        <v>254</v>
+        <v>214</v>
       </c>
       <c r="H104" t="s">
-        <v>255</v>
+        <v>215</v>
       </c>
       <c r="I104">
         <v>0</v>
@@ -14716,19 +14476,19 @@
         <v>25</v>
       </c>
       <c r="D105" t="s">
-        <v>536</v>
+        <v>466</v>
       </c>
       <c r="E105" t="s">
-        <v>537</v>
+        <v>467</v>
       </c>
       <c r="F105" t="s">
-        <v>538</v>
+        <v>468</v>
       </c>
       <c r="G105" t="s">
-        <v>539</v>
+        <v>469</v>
       </c>
       <c r="H105" t="s">
-        <v>540</v>
+        <v>470</v>
       </c>
       <c r="I105">
         <v>0</v>
@@ -14829,19 +14589,19 @@
         <v>25</v>
       </c>
       <c r="D106" t="s">
-        <v>316</v>
+        <v>266</v>
       </c>
       <c r="E106" t="s">
-        <v>317</v>
+        <v>267</v>
       </c>
       <c r="F106" t="s">
-        <v>318</v>
+        <v>268</v>
       </c>
       <c r="G106" t="s">
-        <v>319</v>
+        <v>269</v>
       </c>
       <c r="H106" t="s">
-        <v>320</v>
+        <v>270</v>
       </c>
       <c r="I106">
         <v>0</v>
@@ -14951,19 +14711,19 @@
         <v>25</v>
       </c>
       <c r="D107" t="s">
-        <v>246</v>
+        <v>206</v>
       </c>
       <c r="E107" t="s">
-        <v>247</v>
+        <v>207</v>
       </c>
       <c r="F107" t="s">
-        <v>248</v>
+        <v>208</v>
       </c>
       <c r="G107" t="s">
-        <v>249</v>
+        <v>209</v>
       </c>
       <c r="H107" t="s">
-        <v>250</v>
+        <v>210</v>
       </c>
       <c r="I107">
         <v>0</v>
@@ -15052,19 +14812,19 @@
         <v>25</v>
       </c>
       <c r="D108" t="s">
-        <v>621</v>
+        <v>546</v>
       </c>
       <c r="E108" t="s">
-        <v>622</v>
+        <v>547</v>
       </c>
       <c r="F108" t="s">
-        <v>623</v>
+        <v>548</v>
       </c>
       <c r="G108" t="s">
-        <v>624</v>
+        <v>549</v>
       </c>
       <c r="H108" t="s">
-        <v>625</v>
+        <v>550</v>
       </c>
       <c r="I108">
         <v>0</v>
@@ -15174,19 +14934,19 @@
         <v>25</v>
       </c>
       <c r="D109" t="s">
-        <v>516</v>
+        <v>446</v>
       </c>
       <c r="E109" t="s">
-        <v>517</v>
+        <v>447</v>
       </c>
       <c r="F109" t="s">
-        <v>518</v>
+        <v>448</v>
       </c>
       <c r="G109" t="s">
-        <v>519</v>
+        <v>449</v>
       </c>
       <c r="H109" t="s">
-        <v>520</v>
+        <v>450</v>
       </c>
       <c r="I109">
         <v>0</v>
@@ -15283,1886 +15043,6 @@
       </c>
       <c r="AN109">
         <v>5</v>
-      </c>
-    </row>
-    <row r="110" spans="1:40" x14ac:dyDescent="0.3">
-      <c r="A110" t="b">
-        <v>0</v>
-      </c>
-      <c r="B110" t="s">
-        <v>24</v>
-      </c>
-      <c r="C110" t="s">
-        <v>25</v>
-      </c>
-      <c r="D110" t="s">
-        <v>101</v>
-      </c>
-      <c r="E110" t="s">
-        <v>102</v>
-      </c>
-      <c r="F110" t="s">
-        <v>103</v>
-      </c>
-      <c r="G110" t="s">
-        <v>104</v>
-      </c>
-      <c r="H110" t="s">
-        <v>105</v>
-      </c>
-      <c r="I110">
-        <v>0</v>
-      </c>
-      <c r="J110">
-        <v>33.823999999999998</v>
-      </c>
-      <c r="K110">
-        <v>0</v>
-      </c>
-      <c r="L110">
-        <v>53</v>
-      </c>
-      <c r="M110">
-        <v>3</v>
-      </c>
-      <c r="N110">
-        <v>75</v>
-      </c>
-      <c r="O110">
-        <v>0</v>
-      </c>
-      <c r="P110">
-        <v>2</v>
-      </c>
-      <c r="Q110">
-        <v>112</v>
-      </c>
-      <c r="R110">
-        <v>12</v>
-      </c>
-      <c r="S110">
-        <v>5.34</v>
-      </c>
-      <c r="T110">
-        <v>282.83</v>
-      </c>
-      <c r="U110">
-        <v>53</v>
-      </c>
-      <c r="V110">
-        <v>75</v>
-      </c>
-      <c r="W110">
-        <v>3</v>
-      </c>
-      <c r="X110">
-        <v>0</v>
-      </c>
-      <c r="Y110">
-        <v>8367.8468141801695</v>
-      </c>
-      <c r="Z110">
-        <v>5040.3685293993403</v>
-      </c>
-      <c r="AA110">
-        <v>14806.371908548501</v>
-      </c>
-      <c r="AB110">
-        <v>3523.0028515230101</v>
-      </c>
-      <c r="AC110">
-        <v>10849.4908889823</v>
-      </c>
-      <c r="AD110">
-        <v>13620.5168047227</v>
-      </c>
-      <c r="AE110">
-        <v>17290.936478482901</v>
-      </c>
-      <c r="AF110">
-        <v>17153.6742269754</v>
-      </c>
-      <c r="AG110">
-        <v>1</v>
-      </c>
-      <c r="AH110">
-        <v>1</v>
-      </c>
-      <c r="AK110">
-        <v>1</v>
-      </c>
-      <c r="AM110">
-        <v>1</v>
-      </c>
-      <c r="AN110">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="111" spans="1:40" x14ac:dyDescent="0.3">
-      <c r="A111" t="b">
-        <v>0</v>
-      </c>
-      <c r="B111" t="s">
-        <v>24</v>
-      </c>
-      <c r="C111" t="s">
-        <v>25</v>
-      </c>
-      <c r="D111" t="s">
-        <v>86</v>
-      </c>
-      <c r="E111" t="s">
-        <v>87</v>
-      </c>
-      <c r="F111" t="s">
-        <v>88</v>
-      </c>
-      <c r="G111" t="s">
-        <v>89</v>
-      </c>
-      <c r="H111" t="s">
-        <v>90</v>
-      </c>
-      <c r="I111">
-        <v>0</v>
-      </c>
-      <c r="J111">
-        <v>33.673000000000002</v>
-      </c>
-      <c r="K111">
-        <v>0</v>
-      </c>
-      <c r="L111">
-        <v>14</v>
-      </c>
-      <c r="M111">
-        <v>3</v>
-      </c>
-      <c r="N111">
-        <v>152</v>
-      </c>
-      <c r="O111">
-        <v>3</v>
-      </c>
-      <c r="P111">
-        <v>3</v>
-      </c>
-      <c r="Q111">
-        <v>259</v>
-      </c>
-      <c r="R111">
-        <v>28</v>
-      </c>
-      <c r="S111">
-        <v>6.67</v>
-      </c>
-      <c r="T111">
-        <v>438.76</v>
-      </c>
-      <c r="U111">
-        <v>14</v>
-      </c>
-      <c r="V111">
-        <v>152</v>
-      </c>
-      <c r="W111">
-        <v>3</v>
-      </c>
-      <c r="X111">
-        <v>0</v>
-      </c>
-      <c r="Y111">
-        <v>27448.387784399099</v>
-      </c>
-      <c r="Z111">
-        <v>16059.457152666901</v>
-      </c>
-      <c r="AA111">
-        <v>37856.257020502497</v>
-      </c>
-      <c r="AB111">
-        <v>9744.4802310231298</v>
-      </c>
-      <c r="AC111">
-        <v>14256.5513588578</v>
-      </c>
-      <c r="AD111">
-        <v>27483.525847754601</v>
-      </c>
-      <c r="AE111">
-        <v>16993.377609968898</v>
-      </c>
-      <c r="AF111">
-        <v>14455.580824540601</v>
-      </c>
-      <c r="AG111">
-        <v>1</v>
-      </c>
-      <c r="AH111">
-        <v>1</v>
-      </c>
-      <c r="AI111">
-        <v>2</v>
-      </c>
-      <c r="AJ111">
-        <v>2</v>
-      </c>
-      <c r="AK111">
-        <v>3</v>
-      </c>
-      <c r="AL111">
-        <v>2</v>
-      </c>
-      <c r="AM111">
-        <v>2</v>
-      </c>
-      <c r="AN111">
-        <v>3</v>
-      </c>
-    </row>
-    <row r="112" spans="1:40" x14ac:dyDescent="0.3">
-      <c r="A112" t="b">
-        <v>0</v>
-      </c>
-      <c r="B112" t="s">
-        <v>24</v>
-      </c>
-      <c r="C112" t="s">
-        <v>25</v>
-      </c>
-      <c r="D112" t="s">
-        <v>41</v>
-      </c>
-      <c r="E112" t="s">
-        <v>42</v>
-      </c>
-      <c r="F112" t="s">
-        <v>43</v>
-      </c>
-      <c r="G112" t="s">
-        <v>44</v>
-      </c>
-      <c r="H112" t="s">
-        <v>45</v>
-      </c>
-      <c r="I112">
-        <v>0</v>
-      </c>
-      <c r="J112">
-        <v>33.045999999999999</v>
-      </c>
-      <c r="K112">
-        <v>0</v>
-      </c>
-      <c r="L112">
-        <v>41</v>
-      </c>
-      <c r="M112">
-        <v>5</v>
-      </c>
-      <c r="N112">
-        <v>117</v>
-      </c>
-      <c r="O112">
-        <v>5</v>
-      </c>
-      <c r="P112">
-        <v>5</v>
-      </c>
-      <c r="Q112">
-        <v>88</v>
-      </c>
-      <c r="R112">
-        <v>9.6999999999999993</v>
-      </c>
-      <c r="S112">
-        <v>9.09</v>
-      </c>
-      <c r="T112">
-        <v>241.29</v>
-      </c>
-      <c r="U112">
-        <v>41</v>
-      </c>
-      <c r="V112">
-        <v>117</v>
-      </c>
-      <c r="W112">
-        <v>5</v>
-      </c>
-      <c r="X112">
-        <v>0</v>
-      </c>
-      <c r="Y112">
-        <v>992.99009993612799</v>
-      </c>
-      <c r="Z112">
-        <v>993.38835654780303</v>
-      </c>
-      <c r="AA112">
-        <v>607.02685858196003</v>
-      </c>
-      <c r="AB112">
-        <v>1568.6628860723999</v>
-      </c>
-      <c r="AC112">
-        <v>1638.8855308592299</v>
-      </c>
-      <c r="AD112">
-        <v>3542.3999876247299</v>
-      </c>
-      <c r="AE112">
-        <v>1760.49305416673</v>
-      </c>
-      <c r="AG112">
-        <v>3</v>
-      </c>
-      <c r="AH112">
-        <v>4</v>
-      </c>
-      <c r="AI112">
-        <v>3</v>
-      </c>
-      <c r="AJ112">
-        <v>2</v>
-      </c>
-      <c r="AK112">
-        <v>4</v>
-      </c>
-      <c r="AL112">
-        <v>5</v>
-      </c>
-      <c r="AM112">
-        <v>5</v>
-      </c>
-      <c r="AN112">
-        <v>5</v>
-      </c>
-    </row>
-    <row r="113" spans="1:40" x14ac:dyDescent="0.3">
-      <c r="A113" t="b">
-        <v>0</v>
-      </c>
-      <c r="B113" t="s">
-        <v>24</v>
-      </c>
-      <c r="C113" t="s">
-        <v>25</v>
-      </c>
-      <c r="D113" t="s">
-        <v>306</v>
-      </c>
-      <c r="E113" t="s">
-        <v>307</v>
-      </c>
-      <c r="F113" t="s">
-        <v>308</v>
-      </c>
-      <c r="G113" t="s">
-        <v>309</v>
-      </c>
-      <c r="H113" t="s">
-        <v>310</v>
-      </c>
-      <c r="I113">
-        <v>0</v>
-      </c>
-      <c r="J113">
-        <v>32.865000000000002</v>
-      </c>
-      <c r="K113">
-        <v>0</v>
-      </c>
-      <c r="L113">
-        <v>32</v>
-      </c>
-      <c r="M113">
-        <v>3</v>
-      </c>
-      <c r="N113">
-        <v>75</v>
-      </c>
-      <c r="O113">
-        <v>2</v>
-      </c>
-      <c r="P113">
-        <v>2</v>
-      </c>
-      <c r="Q113">
-        <v>111</v>
-      </c>
-      <c r="R113">
-        <v>12.1</v>
-      </c>
-      <c r="S113">
-        <v>5.38</v>
-      </c>
-      <c r="T113">
-        <v>279.26</v>
-      </c>
-      <c r="U113">
-        <v>32</v>
-      </c>
-      <c r="V113">
-        <v>75</v>
-      </c>
-      <c r="W113">
-        <v>3</v>
-      </c>
-      <c r="X113">
-        <v>1</v>
-      </c>
-      <c r="Y113">
-        <v>205001.77103584999</v>
-      </c>
-      <c r="Z113">
-        <v>67679.092647551704</v>
-      </c>
-      <c r="AA113">
-        <v>65719.559036847902</v>
-      </c>
-      <c r="AB113">
-        <v>90521.946009077903</v>
-      </c>
-      <c r="AC113">
-        <v>115719.933157641</v>
-      </c>
-      <c r="AD113">
-        <v>159501.353002883</v>
-      </c>
-      <c r="AE113">
-        <v>104229.05735394399</v>
-      </c>
-      <c r="AF113">
-        <v>190720.873767048</v>
-      </c>
-      <c r="AG113">
-        <v>3</v>
-      </c>
-      <c r="AH113">
-        <v>2</v>
-      </c>
-      <c r="AI113">
-        <v>3</v>
-      </c>
-      <c r="AJ113">
-        <v>2</v>
-      </c>
-      <c r="AK113">
-        <v>3</v>
-      </c>
-      <c r="AL113">
-        <v>3</v>
-      </c>
-      <c r="AM113">
-        <v>3</v>
-      </c>
-      <c r="AN113">
-        <v>3</v>
-      </c>
-    </row>
-    <row r="114" spans="1:40" x14ac:dyDescent="0.3">
-      <c r="A114" t="b">
-        <v>0</v>
-      </c>
-      <c r="B114" t="s">
-        <v>24</v>
-      </c>
-      <c r="C114" t="s">
-        <v>25</v>
-      </c>
-      <c r="D114" t="s">
-        <v>416</v>
-      </c>
-      <c r="E114" t="s">
-        <v>417</v>
-      </c>
-      <c r="F114" t="s">
-        <v>418</v>
-      </c>
-      <c r="G114" t="s">
-        <v>419</v>
-      </c>
-      <c r="H114" t="s">
-        <v>420</v>
-      </c>
-      <c r="I114">
-        <v>0</v>
-      </c>
-      <c r="J114">
-        <v>32.802</v>
-      </c>
-      <c r="K114">
-        <v>0</v>
-      </c>
-      <c r="L114">
-        <v>11</v>
-      </c>
-      <c r="M114">
-        <v>6</v>
-      </c>
-      <c r="N114">
-        <v>26</v>
-      </c>
-      <c r="O114">
-        <v>6</v>
-      </c>
-      <c r="P114">
-        <v>6</v>
-      </c>
-      <c r="Q114">
-        <v>760</v>
-      </c>
-      <c r="R114">
-        <v>84.7</v>
-      </c>
-      <c r="S114">
-        <v>7.56</v>
-      </c>
-      <c r="T114">
-        <v>54.25</v>
-      </c>
-      <c r="U114">
-        <v>11</v>
-      </c>
-      <c r="V114">
-        <v>26</v>
-      </c>
-      <c r="W114">
-        <v>6</v>
-      </c>
-      <c r="X114">
-        <v>0</v>
-      </c>
-      <c r="Y114">
-        <v>198500.87623724001</v>
-      </c>
-      <c r="Z114">
-        <v>90944.529752336399</v>
-      </c>
-      <c r="AA114">
-        <v>140054.607425928</v>
-      </c>
-      <c r="AB114">
-        <v>63439.265496319502</v>
-      </c>
-      <c r="AC114">
-        <v>130011.875435378</v>
-      </c>
-      <c r="AD114">
-        <v>108610.055909138</v>
-      </c>
-      <c r="AE114">
-        <v>136955.09859702701</v>
-      </c>
-      <c r="AF114">
-        <v>103018.310394071</v>
-      </c>
-      <c r="AG114">
-        <v>3</v>
-      </c>
-      <c r="AH114">
-        <v>1</v>
-      </c>
-      <c r="AI114">
-        <v>2</v>
-      </c>
-      <c r="AJ114">
-        <v>4</v>
-      </c>
-      <c r="AK114">
-        <v>1</v>
-      </c>
-      <c r="AL114">
-        <v>4</v>
-      </c>
-      <c r="AM114">
-        <v>4</v>
-      </c>
-      <c r="AN114">
-        <v>5</v>
-      </c>
-    </row>
-    <row r="115" spans="1:40" x14ac:dyDescent="0.3">
-      <c r="A115" t="b">
-        <v>0</v>
-      </c>
-      <c r="B115" t="s">
-        <v>24</v>
-      </c>
-      <c r="C115" t="s">
-        <v>25</v>
-      </c>
-      <c r="D115" t="s">
-        <v>166</v>
-      </c>
-      <c r="E115" t="s">
-        <v>167</v>
-      </c>
-      <c r="F115" t="s">
-        <v>168</v>
-      </c>
-      <c r="G115" t="s">
-        <v>169</v>
-      </c>
-      <c r="H115" t="s">
-        <v>170</v>
-      </c>
-      <c r="I115">
-        <v>0</v>
-      </c>
-      <c r="J115">
-        <v>32.408999999999999</v>
-      </c>
-      <c r="K115">
-        <v>0</v>
-      </c>
-      <c r="L115">
-        <v>22</v>
-      </c>
-      <c r="M115">
-        <v>4</v>
-      </c>
-      <c r="N115">
-        <v>57</v>
-      </c>
-      <c r="O115">
-        <v>4</v>
-      </c>
-      <c r="P115">
-        <v>4</v>
-      </c>
-      <c r="Q115">
-        <v>263</v>
-      </c>
-      <c r="R115">
-        <v>29.5</v>
-      </c>
-      <c r="S115">
-        <v>6.46</v>
-      </c>
-      <c r="T115">
-        <v>86.18</v>
-      </c>
-      <c r="U115">
-        <v>22</v>
-      </c>
-      <c r="V115">
-        <v>57</v>
-      </c>
-      <c r="W115">
-        <v>4</v>
-      </c>
-      <c r="X115">
-        <v>0</v>
-      </c>
-      <c r="Y115">
-        <v>87808.044085378206</v>
-      </c>
-      <c r="Z115">
-        <v>101889.648276486</v>
-      </c>
-      <c r="AA115">
-        <v>140011.44653876501</v>
-      </c>
-      <c r="AB115">
-        <v>74544.900202236298</v>
-      </c>
-      <c r="AC115">
-        <v>158779.22320681799</v>
-      </c>
-      <c r="AD115">
-        <v>113899.445231684</v>
-      </c>
-      <c r="AE115">
-        <v>165410.94002035301</v>
-      </c>
-      <c r="AF115">
-        <v>157145.78179520401</v>
-      </c>
-      <c r="AG115">
-        <v>1</v>
-      </c>
-      <c r="AH115">
-        <v>2</v>
-      </c>
-      <c r="AI115">
-        <v>4</v>
-      </c>
-      <c r="AJ115">
-        <v>3</v>
-      </c>
-      <c r="AK115">
-        <v>2</v>
-      </c>
-      <c r="AL115">
-        <v>4</v>
-      </c>
-      <c r="AM115">
-        <v>4</v>
-      </c>
-      <c r="AN115">
-        <v>4</v>
-      </c>
-    </row>
-    <row r="116" spans="1:40" x14ac:dyDescent="0.3">
-      <c r="A116" t="b">
-        <v>0</v>
-      </c>
-      <c r="B116" t="s">
-        <v>24</v>
-      </c>
-      <c r="C116" t="s">
-        <v>25</v>
-      </c>
-      <c r="D116" t="s">
-        <v>111</v>
-      </c>
-      <c r="E116" t="s">
-        <v>112</v>
-      </c>
-      <c r="F116" t="s">
-        <v>113</v>
-      </c>
-      <c r="G116" t="s">
-        <v>114</v>
-      </c>
-      <c r="H116" t="s">
-        <v>115</v>
-      </c>
-      <c r="I116">
-        <v>0</v>
-      </c>
-      <c r="J116">
-        <v>31.632999999999999</v>
-      </c>
-      <c r="K116">
-        <v>0</v>
-      </c>
-      <c r="L116">
-        <v>11</v>
-      </c>
-      <c r="M116">
-        <v>3</v>
-      </c>
-      <c r="N116">
-        <v>22</v>
-      </c>
-      <c r="O116">
-        <v>3</v>
-      </c>
-      <c r="P116">
-        <v>3</v>
-      </c>
-      <c r="Q116">
-        <v>251</v>
-      </c>
-      <c r="R116">
-        <v>27.4</v>
-      </c>
-      <c r="S116">
-        <v>6.84</v>
-      </c>
-      <c r="T116">
-        <v>69.36</v>
-      </c>
-      <c r="U116">
-        <v>11</v>
-      </c>
-      <c r="V116">
-        <v>22</v>
-      </c>
-      <c r="W116">
-        <v>3</v>
-      </c>
-      <c r="X116">
-        <v>0</v>
-      </c>
-      <c r="Y116">
-        <v>21183.513066903499</v>
-      </c>
-      <c r="Z116">
-        <v>60653.817202030099</v>
-      </c>
-      <c r="AA116">
-        <v>14456.2984605521</v>
-      </c>
-      <c r="AB116">
-        <v>51852.370276793801</v>
-      </c>
-      <c r="AC116">
-        <v>7302.7703089730403</v>
-      </c>
-      <c r="AD116">
-        <v>17976.806250884401</v>
-      </c>
-      <c r="AE116">
-        <v>36954.169734372197</v>
-      </c>
-      <c r="AF116">
-        <v>50025.827331627901</v>
-      </c>
-      <c r="AH116">
-        <v>1</v>
-      </c>
-      <c r="AI116">
-        <v>2</v>
-      </c>
-      <c r="AJ116">
-        <v>2</v>
-      </c>
-      <c r="AK116">
-        <v>2</v>
-      </c>
-      <c r="AL116">
-        <v>3</v>
-      </c>
-      <c r="AM116">
-        <v>3</v>
-      </c>
-      <c r="AN116">
-        <v>3</v>
-      </c>
-    </row>
-    <row r="117" spans="1:40" x14ac:dyDescent="0.3">
-      <c r="A117" t="b">
-        <v>0</v>
-      </c>
-      <c r="B117" t="s">
-        <v>24</v>
-      </c>
-      <c r="C117" t="s">
-        <v>25</v>
-      </c>
-      <c r="D117" t="s">
-        <v>541</v>
-      </c>
-      <c r="E117" t="s">
-        <v>542</v>
-      </c>
-      <c r="F117" t="s">
-        <v>543</v>
-      </c>
-      <c r="G117" t="s">
-        <v>544</v>
-      </c>
-      <c r="H117" t="s">
-        <v>545</v>
-      </c>
-      <c r="I117">
-        <v>0</v>
-      </c>
-      <c r="J117">
-        <v>29.562000000000001</v>
-      </c>
-      <c r="K117">
-        <v>0</v>
-      </c>
-      <c r="L117">
-        <v>5</v>
-      </c>
-      <c r="M117">
-        <v>4</v>
-      </c>
-      <c r="N117">
-        <v>20</v>
-      </c>
-      <c r="O117">
-        <v>1</v>
-      </c>
-      <c r="P117">
-        <v>4</v>
-      </c>
-      <c r="Q117">
-        <v>963</v>
-      </c>
-      <c r="R117">
-        <v>106.3</v>
-      </c>
-      <c r="S117">
-        <v>4.67</v>
-      </c>
-      <c r="T117">
-        <v>40.76</v>
-      </c>
-      <c r="U117">
-        <v>5</v>
-      </c>
-      <c r="V117">
-        <v>20</v>
-      </c>
-      <c r="W117">
-        <v>4</v>
-      </c>
-      <c r="X117">
-        <v>0</v>
-      </c>
-      <c r="AC117">
-        <v>2706.4614182943101</v>
-      </c>
-      <c r="AD117">
-        <v>1433.5255768413799</v>
-      </c>
-      <c r="AE117">
-        <v>2938.4177425684002</v>
-      </c>
-      <c r="AF117">
-        <v>2757.7056066596501</v>
-      </c>
-      <c r="AG117">
-        <v>1</v>
-      </c>
-      <c r="AH117">
-        <v>1</v>
-      </c>
-      <c r="AI117">
-        <v>2</v>
-      </c>
-      <c r="AJ117">
-        <v>2</v>
-      </c>
-      <c r="AK117">
-        <v>2</v>
-      </c>
-      <c r="AL117">
-        <v>3</v>
-      </c>
-      <c r="AM117">
-        <v>3</v>
-      </c>
-      <c r="AN117">
-        <v>2</v>
-      </c>
-    </row>
-    <row r="118" spans="1:40" x14ac:dyDescent="0.3">
-      <c r="A118" t="b">
-        <v>0</v>
-      </c>
-      <c r="B118" t="s">
-        <v>24</v>
-      </c>
-      <c r="C118" t="s">
-        <v>25</v>
-      </c>
-      <c r="D118" t="s">
-        <v>341</v>
-      </c>
-      <c r="E118" t="s">
-        <v>342</v>
-      </c>
-      <c r="F118" t="s">
-        <v>343</v>
-      </c>
-      <c r="G118" t="s">
-        <v>344</v>
-      </c>
-      <c r="H118" t="s">
-        <v>345</v>
-      </c>
-      <c r="I118">
-        <v>0</v>
-      </c>
-      <c r="J118">
-        <v>29.484000000000002</v>
-      </c>
-      <c r="K118">
-        <v>0</v>
-      </c>
-      <c r="L118">
-        <v>10</v>
-      </c>
-      <c r="M118">
-        <v>6</v>
-      </c>
-      <c r="N118">
-        <v>40</v>
-      </c>
-      <c r="O118">
-        <v>6</v>
-      </c>
-      <c r="P118">
-        <v>6</v>
-      </c>
-      <c r="Q118">
-        <v>623</v>
-      </c>
-      <c r="R118">
-        <v>67.599999999999994</v>
-      </c>
-      <c r="S118">
-        <v>7.5</v>
-      </c>
-      <c r="T118">
-        <v>48.02</v>
-      </c>
-      <c r="U118">
-        <v>10</v>
-      </c>
-      <c r="V118">
-        <v>40</v>
-      </c>
-      <c r="W118">
-        <v>6</v>
-      </c>
-      <c r="X118">
-        <v>0</v>
-      </c>
-      <c r="Y118">
-        <v>7136.2791558258205</v>
-      </c>
-      <c r="Z118">
-        <v>11902.6322050989</v>
-      </c>
-      <c r="AA118">
-        <v>9444.4173434713503</v>
-      </c>
-      <c r="AB118">
-        <v>11218.2132408835</v>
-      </c>
-      <c r="AC118">
-        <v>32361.171524091798</v>
-      </c>
-      <c r="AD118">
-        <v>38477.169571071099</v>
-      </c>
-      <c r="AE118">
-        <v>68942.103462720697</v>
-      </c>
-      <c r="AF118">
-        <v>50088.241340184199</v>
-      </c>
-      <c r="AG118">
-        <v>3</v>
-      </c>
-      <c r="AH118">
-        <v>3</v>
-      </c>
-      <c r="AI118">
-        <v>4</v>
-      </c>
-      <c r="AJ118">
-        <v>3</v>
-      </c>
-      <c r="AK118">
-        <v>4</v>
-      </c>
-      <c r="AL118">
-        <v>5</v>
-      </c>
-      <c r="AM118">
-        <v>5</v>
-      </c>
-      <c r="AN118">
-        <v>5</v>
-      </c>
-    </row>
-    <row r="119" spans="1:40" x14ac:dyDescent="0.3">
-      <c r="A119" t="b">
-        <v>0</v>
-      </c>
-      <c r="B119" t="s">
-        <v>24</v>
-      </c>
-      <c r="C119" t="s">
-        <v>25</v>
-      </c>
-      <c r="D119" t="s">
-        <v>56</v>
-      </c>
-      <c r="E119" t="s">
-        <v>57</v>
-      </c>
-      <c r="F119" t="s">
-        <v>58</v>
-      </c>
-      <c r="G119" t="s">
-        <v>59</v>
-      </c>
-      <c r="H119" t="s">
-        <v>60</v>
-      </c>
-      <c r="I119">
-        <v>0</v>
-      </c>
-      <c r="J119">
-        <v>29.289000000000001</v>
-      </c>
-      <c r="K119">
-        <v>0</v>
-      </c>
-      <c r="L119">
-        <v>8</v>
-      </c>
-      <c r="M119">
-        <v>5</v>
-      </c>
-      <c r="N119">
-        <v>24</v>
-      </c>
-      <c r="O119">
-        <v>5</v>
-      </c>
-      <c r="P119">
-        <v>5</v>
-      </c>
-      <c r="Q119">
-        <v>1066</v>
-      </c>
-      <c r="R119">
-        <v>116.6</v>
-      </c>
-      <c r="S119">
-        <v>6</v>
-      </c>
-      <c r="T119">
-        <v>52.6</v>
-      </c>
-      <c r="U119">
-        <v>8</v>
-      </c>
-      <c r="V119">
-        <v>24</v>
-      </c>
-      <c r="W119">
-        <v>5</v>
-      </c>
-      <c r="X119">
-        <v>0</v>
-      </c>
-      <c r="Y119">
-        <v>6641.4386459429597</v>
-      </c>
-      <c r="Z119">
-        <v>4002.3888884918401</v>
-      </c>
-      <c r="AA119">
-        <v>4645.4958640438299</v>
-      </c>
-      <c r="AB119">
-        <v>5872.1819120329601</v>
-      </c>
-      <c r="AC119">
-        <v>6239.79933023185</v>
-      </c>
-      <c r="AD119">
-        <v>10338.9690365106</v>
-      </c>
-      <c r="AE119">
-        <v>9903.5550350984904</v>
-      </c>
-      <c r="AF119">
-        <v>7445.0512141531699</v>
-      </c>
-      <c r="AG119">
-        <v>1</v>
-      </c>
-      <c r="AH119">
-        <v>3</v>
-      </c>
-      <c r="AI119">
-        <v>3</v>
-      </c>
-      <c r="AJ119">
-        <v>3</v>
-      </c>
-      <c r="AK119">
-        <v>2</v>
-      </c>
-      <c r="AL119">
-        <v>4</v>
-      </c>
-      <c r="AM119">
-        <v>4</v>
-      </c>
-      <c r="AN119">
-        <v>4</v>
-      </c>
-    </row>
-    <row r="120" spans="1:40" x14ac:dyDescent="0.3">
-      <c r="A120" t="b">
-        <v>0</v>
-      </c>
-      <c r="B120" t="s">
-        <v>24</v>
-      </c>
-      <c r="C120" t="s">
-        <v>25</v>
-      </c>
-      <c r="D120" t="s">
-        <v>441</v>
-      </c>
-      <c r="E120" t="s">
-        <v>442</v>
-      </c>
-      <c r="F120" t="s">
-        <v>443</v>
-      </c>
-      <c r="G120" t="s">
-        <v>444</v>
-      </c>
-      <c r="H120" t="s">
-        <v>445</v>
-      </c>
-      <c r="I120">
-        <v>0</v>
-      </c>
-      <c r="J120">
-        <v>29.096</v>
-      </c>
-      <c r="K120">
-        <v>0</v>
-      </c>
-      <c r="L120">
-        <v>8</v>
-      </c>
-      <c r="M120">
-        <v>5</v>
-      </c>
-      <c r="N120">
-        <v>419</v>
-      </c>
-      <c r="O120">
-        <v>1</v>
-      </c>
-      <c r="P120">
-        <v>2</v>
-      </c>
-      <c r="Q120">
-        <v>565</v>
-      </c>
-      <c r="R120">
-        <v>62.6</v>
-      </c>
-      <c r="S120">
-        <v>6</v>
-      </c>
-      <c r="T120">
-        <v>586.39</v>
-      </c>
-      <c r="U120">
-        <v>8</v>
-      </c>
-      <c r="V120">
-        <v>419</v>
-      </c>
-      <c r="W120">
-        <v>5</v>
-      </c>
-      <c r="X120">
-        <v>0</v>
-      </c>
-      <c r="Y120">
-        <v>1583.9058538271499</v>
-      </c>
-      <c r="Z120">
-        <v>4238.9826155225901</v>
-      </c>
-      <c r="AA120">
-        <v>1693.7762391988899</v>
-      </c>
-      <c r="AB120">
-        <v>570.50214988452205</v>
-      </c>
-      <c r="AC120">
-        <v>3501.11892051309</v>
-      </c>
-      <c r="AD120">
-        <v>5793.9402127608701</v>
-      </c>
-      <c r="AE120">
-        <v>8366.4180770684798</v>
-      </c>
-      <c r="AF120">
-        <v>1607.9965501403799</v>
-      </c>
-      <c r="AH120">
-        <v>1</v>
-      </c>
-      <c r="AK120">
-        <v>1</v>
-      </c>
-      <c r="AL120">
-        <v>1</v>
-      </c>
-      <c r="AN120">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="121" spans="1:40" x14ac:dyDescent="0.3">
-      <c r="A121" t="b">
-        <v>0</v>
-      </c>
-      <c r="B121" t="s">
-        <v>24</v>
-      </c>
-      <c r="C121" t="s">
-        <v>25</v>
-      </c>
-      <c r="D121" t="s">
-        <v>146</v>
-      </c>
-      <c r="E121" t="s">
-        <v>147</v>
-      </c>
-      <c r="F121" t="s">
-        <v>148</v>
-      </c>
-      <c r="G121" t="s">
-        <v>149</v>
-      </c>
-      <c r="H121" t="s">
-        <v>150</v>
-      </c>
-      <c r="I121">
-        <v>0</v>
-      </c>
-      <c r="J121">
-        <v>28.434000000000001</v>
-      </c>
-      <c r="K121">
-        <v>0</v>
-      </c>
-      <c r="L121">
-        <v>27</v>
-      </c>
-      <c r="M121">
-        <v>5</v>
-      </c>
-      <c r="N121">
-        <v>58</v>
-      </c>
-      <c r="O121">
-        <v>3</v>
-      </c>
-      <c r="P121">
-        <v>5</v>
-      </c>
-      <c r="Q121">
-        <v>254</v>
-      </c>
-      <c r="R121">
-        <v>28.8</v>
-      </c>
-      <c r="S121">
-        <v>7.18</v>
-      </c>
-      <c r="T121">
-        <v>77.099999999999994</v>
-      </c>
-      <c r="U121">
-        <v>27</v>
-      </c>
-      <c r="V121">
-        <v>58</v>
-      </c>
-      <c r="W121">
-        <v>5</v>
-      </c>
-      <c r="X121">
-        <v>0</v>
-      </c>
-      <c r="Z121">
-        <v>6809.4123084418497</v>
-      </c>
-      <c r="AC121">
-        <v>2800.6634968830599</v>
-      </c>
-      <c r="AD121">
-        <v>1586.97997948125</v>
-      </c>
-      <c r="AE121">
-        <v>1677.98960082337</v>
-      </c>
-      <c r="AF121">
-        <v>559.44202075153601</v>
-      </c>
-      <c r="AG121">
-        <v>4</v>
-      </c>
-      <c r="AH121">
-        <v>3</v>
-      </c>
-      <c r="AI121">
-        <v>3</v>
-      </c>
-      <c r="AJ121">
-        <v>4</v>
-      </c>
-      <c r="AK121">
-        <v>3</v>
-      </c>
-      <c r="AL121">
-        <v>4</v>
-      </c>
-      <c r="AM121">
-        <v>4</v>
-      </c>
-      <c r="AN121">
-        <v>4</v>
-      </c>
-    </row>
-    <row r="122" spans="1:40" x14ac:dyDescent="0.3">
-      <c r="A122" t="b">
-        <v>0</v>
-      </c>
-      <c r="B122" t="s">
-        <v>24</v>
-      </c>
-      <c r="C122" t="s">
-        <v>25</v>
-      </c>
-      <c r="D122" t="s">
-        <v>291</v>
-      </c>
-      <c r="E122" t="s">
-        <v>292</v>
-      </c>
-      <c r="F122" t="s">
-        <v>293</v>
-      </c>
-      <c r="G122" t="s">
-        <v>294</v>
-      </c>
-      <c r="H122" t="s">
-        <v>295</v>
-      </c>
-      <c r="I122">
-        <v>0</v>
-      </c>
-      <c r="J122">
-        <v>27.734000000000002</v>
-      </c>
-      <c r="K122">
-        <v>0</v>
-      </c>
-      <c r="L122">
-        <v>5</v>
-      </c>
-      <c r="M122">
-        <v>2</v>
-      </c>
-      <c r="N122">
-        <v>30</v>
-      </c>
-      <c r="O122">
-        <v>2</v>
-      </c>
-      <c r="P122">
-        <v>2</v>
-      </c>
-      <c r="Q122">
-        <v>685</v>
-      </c>
-      <c r="R122">
-        <v>75.5</v>
-      </c>
-      <c r="S122">
-        <v>6.07</v>
-      </c>
-      <c r="T122">
-        <v>88.04</v>
-      </c>
-      <c r="U122">
-        <v>5</v>
-      </c>
-      <c r="V122">
-        <v>30</v>
-      </c>
-      <c r="W122">
-        <v>2</v>
-      </c>
-      <c r="X122">
-        <v>0</v>
-      </c>
-      <c r="Y122">
-        <v>319.62545137947802</v>
-      </c>
-      <c r="Z122">
-        <v>178.13719297549099</v>
-      </c>
-      <c r="AA122">
-        <v>692.93398560988896</v>
-      </c>
-      <c r="AC122">
-        <v>861.12198740652195</v>
-      </c>
-      <c r="AD122">
-        <v>1869.2487585246599</v>
-      </c>
-      <c r="AE122">
-        <v>1945.1650228326</v>
-      </c>
-      <c r="AF122">
-        <v>2142.2283153082099</v>
-      </c>
-      <c r="AG122">
-        <v>2</v>
-      </c>
-      <c r="AH122">
-        <v>1</v>
-      </c>
-      <c r="AI122">
-        <v>2</v>
-      </c>
-      <c r="AJ122">
-        <v>2</v>
-      </c>
-      <c r="AK122">
-        <v>1</v>
-      </c>
-      <c r="AL122">
-        <v>2</v>
-      </c>
-      <c r="AM122">
-        <v>2</v>
-      </c>
-      <c r="AN122">
-        <v>2</v>
-      </c>
-    </row>
-    <row r="123" spans="1:40" x14ac:dyDescent="0.3">
-      <c r="A123" t="b">
-        <v>0</v>
-      </c>
-      <c r="B123" t="s">
-        <v>24</v>
-      </c>
-      <c r="C123" t="s">
-        <v>25</v>
-      </c>
-      <c r="D123" t="s">
-        <v>636</v>
-      </c>
-      <c r="E123" t="s">
-        <v>637</v>
-      </c>
-      <c r="F123" t="s">
-        <v>638</v>
-      </c>
-      <c r="G123" t="s">
-        <v>639</v>
-      </c>
-      <c r="H123" t="s">
-        <v>640</v>
-      </c>
-      <c r="I123">
-        <v>0</v>
-      </c>
-      <c r="J123">
-        <v>27.22</v>
-      </c>
-      <c r="K123">
-        <v>0</v>
-      </c>
-      <c r="L123">
-        <v>19</v>
-      </c>
-      <c r="M123">
-        <v>3</v>
-      </c>
-      <c r="N123">
-        <v>40</v>
-      </c>
-      <c r="O123">
-        <v>3</v>
-      </c>
-      <c r="P123">
-        <v>3</v>
-      </c>
-      <c r="Q123">
-        <v>245</v>
-      </c>
-      <c r="R123">
-        <v>26</v>
-      </c>
-      <c r="S123">
-        <v>9.11</v>
-      </c>
-      <c r="T123">
-        <v>71.28</v>
-      </c>
-      <c r="U123">
-        <v>19</v>
-      </c>
-      <c r="V123">
-        <v>40</v>
-      </c>
-      <c r="W123">
-        <v>3</v>
-      </c>
-      <c r="X123">
-        <v>0</v>
-      </c>
-      <c r="Y123">
-        <v>27880.0639339298</v>
-      </c>
-      <c r="Z123">
-        <v>22304.683380263999</v>
-      </c>
-      <c r="AA123">
-        <v>28599.792353167399</v>
-      </c>
-      <c r="AB123">
-        <v>31108.237106061701</v>
-      </c>
-      <c r="AC123">
-        <v>37687.567591979401</v>
-      </c>
-      <c r="AD123">
-        <v>16593.021143259899</v>
-      </c>
-      <c r="AE123">
-        <v>24230.455129025901</v>
-      </c>
-      <c r="AF123">
-        <v>29560.171988043199</v>
-      </c>
-      <c r="AG123">
-        <v>3</v>
-      </c>
-      <c r="AH123">
-        <v>3</v>
-      </c>
-      <c r="AI123">
-        <v>2</v>
-      </c>
-      <c r="AJ123">
-        <v>3</v>
-      </c>
-      <c r="AK123">
-        <v>2</v>
-      </c>
-      <c r="AL123">
-        <v>3</v>
-      </c>
-      <c r="AM123">
-        <v>3</v>
-      </c>
-      <c r="AN123">
-        <v>3</v>
-      </c>
-    </row>
-    <row r="124" spans="1:40" x14ac:dyDescent="0.3">
-      <c r="A124" t="b">
-        <v>0</v>
-      </c>
-      <c r="B124" t="s">
-        <v>24</v>
-      </c>
-      <c r="C124" t="s">
-        <v>25</v>
-      </c>
-      <c r="D124" t="s">
-        <v>421</v>
-      </c>
-      <c r="E124" t="s">
-        <v>422</v>
-      </c>
-      <c r="F124" t="s">
-        <v>423</v>
-      </c>
-      <c r="G124" t="s">
-        <v>424</v>
-      </c>
-      <c r="H124" t="s">
-        <v>425</v>
-      </c>
-      <c r="I124">
-        <v>0</v>
-      </c>
-      <c r="J124">
-        <v>26.504999999999999</v>
-      </c>
-      <c r="K124">
-        <v>0</v>
-      </c>
-      <c r="L124">
-        <v>3</v>
-      </c>
-      <c r="M124">
-        <v>2</v>
-      </c>
-      <c r="N124">
-        <v>15</v>
-      </c>
-      <c r="O124">
-        <v>2</v>
-      </c>
-      <c r="P124">
-        <v>2</v>
-      </c>
-      <c r="Q124">
-        <v>493</v>
-      </c>
-      <c r="R124">
-        <v>54.4</v>
-      </c>
-      <c r="S124">
-        <v>6.62</v>
-      </c>
-      <c r="T124">
-        <v>42.79</v>
-      </c>
-      <c r="U124">
-        <v>3</v>
-      </c>
-      <c r="V124">
-        <v>15</v>
-      </c>
-      <c r="W124">
-        <v>2</v>
-      </c>
-      <c r="X124">
-        <v>0</v>
-      </c>
-      <c r="AE124">
-        <v>437.427723638982</v>
-      </c>
-      <c r="AG124">
-        <v>1</v>
-      </c>
-      <c r="AH124">
-        <v>1</v>
-      </c>
-      <c r="AI124">
-        <v>1</v>
-      </c>
-      <c r="AJ124">
-        <v>1</v>
-      </c>
-      <c r="AK124">
-        <v>1</v>
-      </c>
-      <c r="AL124">
-        <v>1</v>
-      </c>
-      <c r="AM124">
-        <v>1</v>
-      </c>
-      <c r="AN124">
-        <v>2</v>
-      </c>
-    </row>
-    <row r="125" spans="1:40" x14ac:dyDescent="0.3">
-      <c r="A125" t="b">
-        <v>0</v>
-      </c>
-      <c r="B125" t="s">
-        <v>24</v>
-      </c>
-      <c r="C125" t="s">
-        <v>25</v>
-      </c>
-      <c r="D125" t="s">
-        <v>176</v>
-      </c>
-      <c r="E125" t="s">
-        <v>177</v>
-      </c>
-      <c r="F125" t="s">
-        <v>178</v>
-      </c>
-      <c r="G125" t="s">
-        <v>179</v>
-      </c>
-      <c r="H125" t="s">
-        <v>180</v>
-      </c>
-      <c r="I125">
-        <v>0</v>
-      </c>
-      <c r="J125">
-        <v>25.274999999999999</v>
-      </c>
-      <c r="K125">
-        <v>0</v>
-      </c>
-      <c r="L125">
-        <v>7</v>
-      </c>
-      <c r="M125">
-        <v>4</v>
-      </c>
-      <c r="N125">
-        <v>61</v>
-      </c>
-      <c r="O125">
-        <v>4</v>
-      </c>
-      <c r="P125">
-        <v>4</v>
-      </c>
-      <c r="Q125">
-        <v>338</v>
-      </c>
-      <c r="R125">
-        <v>38.200000000000003</v>
-      </c>
-      <c r="S125">
-        <v>6.43</v>
-      </c>
-      <c r="T125">
-        <v>89.48</v>
-      </c>
-      <c r="U125">
-        <v>7</v>
-      </c>
-      <c r="V125">
-        <v>61</v>
-      </c>
-      <c r="W125">
-        <v>4</v>
-      </c>
-      <c r="X125">
-        <v>0</v>
-      </c>
-      <c r="Y125">
-        <v>10357.7187334299</v>
-      </c>
-      <c r="Z125">
-        <v>6561.7595375178798</v>
-      </c>
-      <c r="AA125">
-        <v>5496.4853093111496</v>
-      </c>
-      <c r="AB125">
-        <v>5047.7734043997498</v>
-      </c>
-      <c r="AC125">
-        <v>236254.14759885901</v>
-      </c>
-      <c r="AD125">
-        <v>289198.28840281098</v>
-      </c>
-      <c r="AE125">
-        <v>317355.57973750302</v>
-      </c>
-      <c r="AF125">
-        <v>244903.948614694</v>
-      </c>
-      <c r="AG125">
-        <v>3</v>
-      </c>
-      <c r="AH125">
-        <v>1</v>
-      </c>
-      <c r="AI125">
-        <v>3</v>
-      </c>
-      <c r="AJ125">
-        <v>4</v>
-      </c>
-      <c r="AK125">
-        <v>4</v>
-      </c>
-      <c r="AL125">
-        <v>4</v>
-      </c>
-      <c r="AM125">
-        <v>4</v>
-      </c>
-      <c r="AN125">
-        <v>4</v>
       </c>
     </row>
   </sheetData>

</xml_diff>